<commit_message>
Y1D - Name changes in MS Teams Assignment Template
</commit_message>
<xml_diff>
--- a/docs/Year1/BlockD/MS Assignment Template/Self-Assessment Rubric Block - Y1D_2022-23_ADSAI.xlsx
+++ b/docs/Year1/BlockD/MS Assignment Template/Self-Assessment Rubric Block - Y1D_2022-23_ADSAI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26412"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bramh\Documents\GitHub\AAI-DM\docs\Year1\BlockD\MS Assignment Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://edubuas.sharepoint.com/teams/ADSAI2022-23/Shared Documents/General/Design documentation/Year 1 Design/Block D/MS Teams Assignment Template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA54226-8787-49A8-809E-2B19D1B58E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="678" documentId="11_03746045E4F30D67E4D3283C82E484B242FC1AB4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35BEF582-8A36-474F-B837-16F776521440}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="50910" windowHeight="21840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1068" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Student Self-Assessment" sheetId="6" r:id="rId1"/>
@@ -30,6 +30,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="244">
   <si>
     <t>Student Self-Assessment</t>
   </si>
@@ -82,6 +83,9 @@
     <t>Student Number</t>
   </si>
   <si>
+    <t>Municipality of Breda - Improve Breda</t>
+  </si>
+  <si>
     <t>GRADE</t>
   </si>
   <si>
@@ -91,6 +95,9 @@
     <t>Project</t>
   </si>
   <si>
+    <t>2022-32D FGA1.P4-ADSAI</t>
+  </si>
+  <si>
     <t>Opportunity</t>
   </si>
   <si>
@@ -100,7 +107,7 @@
     <t>Project Deadline</t>
   </si>
   <si>
-    <t>5pm Friday 30th June</t>
+    <t>16:59 Friday 23th June</t>
   </si>
   <si>
     <t>Grading Rubric</t>
@@ -162,13 +169,13 @@
     </r>
   </si>
   <si>
-    <t>1.1 Creates and updates plans to work effectively based on agreed upon priorities with consideration of dependencies and risk, using sound estimates to achieve short and long-term project goals.</t>
+    <t>1.1 Creates and updates plans to work effectively based on agreed upon priorities with consideration of dependencies and risks, using sound estimates to achieve short and long-term project goals.</t>
   </si>
   <si>
     <t>Not addressed this block in your project work. Your project work evidencing can include your Learning Log, Work-log, GitHub commits and supporting documents you submitted with your project by uploading during hand-in.</t>
   </si>
   <si>
-    <t>High level plan (e.g. a roadmap) breaking the project into phases.</t>
+    <t>High level plan (e.g. a roadmap) breaking the project into phases. Clear Individual contribution  is documented.</t>
   </si>
   <si>
     <t xml:space="preserve">Clear tasks and user stories created. And meeting all criteria in poor. </t>
@@ -177,10 +184,10 @@
     <t xml:space="preserve">Project and task planning clearly broken into days/weeks/phases within the project or block.  All project tasks have time/story point estimates. And meeting all criteria in insufficient. </t>
   </si>
   <si>
-    <t xml:space="preserve">Planning is feasible. Risks have been identified. Professional attendance for all classes and team meetings (including stand-ups)  in person. Healthy backlog (or thorough task coverage of possible project directions) maintained. And meeting all criteria in sufficient. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Planning is revisited and adjusted if required during the project. Risks identified have associated risk minimisation or elimination plans that were put into action where possible. Planning also factors in self-development time and how that is spent. And meeting all criteria in good. </t>
+    <t xml:space="preserve">Planning is feasible. Risks have been identified. Professional attendance for all classes and team meetings (including stand-ups). Healthy backlog (or thorough task coverage of possible project directions) maintained. Conducts a project retrospective about what went well, what could have been better, and how to improve in the future. And meeting all criteria in sufficient. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Planning is revisited and adjusted if required during the project. Risks identified have associated risk minimisation or elimination plans that were put into action where possible. Planning also factors in self-development time and how that is spent. Proposes improvements to the deployment plan including action points which are derived from the project retrospective. And meeting all criteria in good. </t>
   </si>
   <si>
     <t>1.4 Regularly and objectively reviews progress on project and team goals and processes, reflecting on the strengths and weaknesses through project and peer reviews.</t>
@@ -204,10 +211,10 @@
     <t>1.5 Communicates productively while effectively adjusting to varied communication styles and intercultural differences in team work.</t>
   </si>
   <si>
-    <t xml:space="preserve">Participates in the communication workshops. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brings issues to the table during standup sessions and/or retrospectives, when neccesary. And meeting all criteria in poor. </t>
+    <t xml:space="preserve">Participates in a communication workshop. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brings issues to the table during standup sessions and/or review/retrospectives, when neccesary. And meeting all criteria in poor. </t>
   </si>
   <si>
     <t xml:space="preserve">Communicates effectively with all stakeholders, evidenced by peer review. And meeting all criteria in insufficient.  </t>
@@ -245,7 +252,7 @@
 Demonstrates self-exploration and personal development, good academic practices in learning how to learn and the acquisition of professional knowledge through research, study, analysis, applied practice, discussion and reporting, where an excellent performance would show:</t>
   </si>
   <si>
-    <t>2.1 Sets ambitious, S.M.A.R.T./ C.L.E.A.R goals in alignment with the project brief, their chosen role(s), content of the assessment rubric and their personal long-term goals.</t>
+    <t>2.1 Sets ambitious, S.M.A.R.T.E.R. goals in alignment with the project brief, content of the assessment rubric and their personal long-term goals.</t>
   </si>
   <si>
     <t>Some project goals and self-development goals detailed.</t>
@@ -268,62 +275,49 @@
   </si>
   <si>
     <t>3.0 Legal
-The student demonstrates the basic knowledge of legal frameworks governing AI by providing evidence of legal decision-making while working with privacy-sensitive data.</t>
-  </si>
-  <si>
-    <t>3.1 Demonstrates the basic knowledge of legal frameworks governing AI by providing evidence of legal decision-making while working with privacy-sensitive data.</t>
+The student demonstrates the basic knowledge of legal and ethical frameworks governing AI by providing evidence of legal and ethical decision-making while working with privacy-sensitive data.</t>
+  </si>
+  <si>
+    <t>3.1 Demonstrates the basic knowledge of legal and ethical frameworks governing AI by providing evidence of legal and ethical decision-making while working with (privacy-)sensitive data.</t>
   </si>
   <si>
     <t xml:space="preserve">Not addressed this block in your project work. Your project work evidencing can include your Learning Log, Work-log, GitHub commits and supporting documents you submitted with your project by uploading during hand-in. </t>
   </si>
   <si>
-    <t>The student attends the debate and contributes to the report.</t>
-  </si>
-  <si>
-    <t>The student is able to create the checklist of legal aspects for the legal inquiry of the project. And meeting all criteria in poor.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The student is able to properly define a thesis statement for the debate. The student is able to provide facts, reasons, examples, explanations, and evidence in data projects. 
-The checklist for legal inquiry of the project is based on the literature provided during the module. The legal aspects important for the project are identified. And meeting all criteria in insufficient.
+    <t>Clear Individual contribution  is documented.</t>
+  </si>
+  <si>
+    <t>The student is able to create a checklist of legal and ethical aspects for the legal and ethical inquiry of the project. And meeting all criteria in poor.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The checklist for legal and ethical inquiry of the project is based on the  DEDA and ALTAI frameworks provided during the module. The legal and ethical aspects important to the project are identified and included into the checklist. The legal and ethical aspects not important for the project are identified and not included into the checklist. The checklist is filled in. And meeting all criteria in insufficient.
 </t>
   </si>
   <si>
-    <t>The student is able to develop argumentation based on important facts, details, examples, and explanations from multiple authoritative sources. The student is able to differentiate facts from opinions and structure ideas and arguments in a sustained and logical fashion. The legal aspects important for the project are interpreted. And meeting all criteria in sufficient.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The student is able to propose improvements of the approach chosen based on argumentation mentioned under "good".  </t>
+    <t xml:space="preserve">The relevance of legal and ethical aspects included in the checklists for this project is explained. The reasoning for not including certain legal and ethical aspects in the checklist is justified. Argumentation for including and excluding legal and ethical aspects for the checklist is based on important facts, details, examples, and explanations from multiple authoritative sources and data.  And meeting all criteria in sufficient. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student provides evidence and explanations of legal and ethical decision-making for aspects within the checklist (where possible). And meeting all criteria in good.  </t>
   </si>
   <si>
     <t>Competency 1,2
 Dublin Descriptors 1, 2, 3,4, 5</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">4.0 Business understanding
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="3"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>The student is able to determine business objectives,  and produce a project plan.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">4.1 The student is able to show understanding of the business understanding phase by writing a project plan. </t>
+    <t>4.0 Business understanding
+The student is able to determine business objectives, produce a project plan and disseminate project results.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.1 The student is able to show understanding of the business understanding phase by writing a project plan and disseminate project results. </t>
   </si>
   <si>
     <t>Clear individual contribution is documented.</t>
   </si>
   <si>
-    <t xml:space="preserve">The project vision and roadmap is present. And meeting all criteria in poor. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shows thorough understanding, from a business perspective, what the client really wants to accomplish, and derives business requirements. And meeting all criteria in insufficient.  </t>
+    <t xml:space="preserve">The project vision, roadmap, and poster is present. And meeting all criteria in poor. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shows thorough understanding, from a business perspective, what the client really wants to accomplish, and derives business requirements. Iterates on the project based on (client) feedback. And meeting all criteria in insufficient.  </t>
   </si>
   <si>
     <t xml:space="preserve">Contributes to determination of resources and tools neccesary to meet business requirements. And meeting all criteria in sufficient. </t>
@@ -355,7 +349,7 @@
     <t xml:space="preserve">Assess the quality of the data, and draft a data quality report. And meeting all criteria in sufficient. </t>
   </si>
   <si>
-    <t xml:space="preserve">Propose improvements to the datamanagement strategy. And meeting all criteria in good. </t>
+    <t xml:space="preserve">Propose improvements to the data management strategy. And meeting all criteria in good. </t>
   </si>
   <si>
     <t>Competencies 5,6
@@ -369,44 +363,41 @@
     <t>6.1 Demonstrates an understanding of the modelling and evaluation stage by developing a model suitable for deployment.</t>
   </si>
   <si>
-    <t>Clear Individual contribution  is documented.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Clear contribution to the selection of appropriate performance metrics is documented. And meeting all criteria in poor. </t>
   </si>
   <si>
     <t xml:space="preserve">Implements the machine learning model, and applies feature engineering (if necessary). And meeting all criteria in insufficient.  </t>
   </si>
   <si>
-    <t xml:space="preserve">Evaluates the model and improves model performance to meet the business criteria if necessary. Documents the work done and ensures code is of production quality. And meeting all criteria in sufficient. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compares multiple models and justify your choice of the final model in the project document. And meeting all criteria in good. </t>
+    <t xml:space="preserve">Evaluates the model and improves model performance to meet the business criteria if necessary. And meeting all criteria in sufficient. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Documents the machine learning lifecycle for the models utilized. And meeting all criteria in good. </t>
   </si>
   <si>
     <t>Competencies 7, 8
 Dublin Descriptors 1, 2, 3, 4, 5</t>
   </si>
   <si>
-    <t xml:space="preserve">7.0 Deployment                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                               Is able to plan deployment, disseminate the project results, produce a final report and review the project.                                                                                                                                                                                                                                                                      </t>
-  </si>
-  <si>
-    <t>7.1 Demonstrates understanding of the deployment stage by disseminating the project findings and conducting a project restrospective.</t>
-  </si>
-  <si>
-    <t>Clear Individual contribution is documented.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The project report is present. And meeting all criteria in poor. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">A plan for deploying the model has been designed and further, contributes to project dissemination. And meeting all criteria in insufficient.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Conducts a project retrospective about what went well, what could have been better, and how to improve in the future. And meeting all criteria in sufficient. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proposes improvements to the deployment plan including action points which are derived from the project retrospective. And meeting all criteria in good. </t>
+    <t xml:space="preserve">7.0 Deployment                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                               Is able to deliver value to the stakeholders and delivering production-ready code that is designed to be implemented into practical real-world scenarios such as applications or products.                                                                                                                                                                                                                                                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.1 Is able to deliver value to the stakeholders and deliver production-ready code that is designed to be implemented into practical real-world scenarios such as applications or products.                </t>
+  </si>
+  <si>
+    <t>Clear Individual contribution is documented. Python scripts are delivered (in place of Jupyter notebooks).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creates a virtual environment and utilizes it alongside a package manager, enabling efficient management of dependencies and packages required for a data science project. And meeting all criteria in poor. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Works towards delivering clean code according to industry standards, for example, by using logging, linting,  doc strings, code formatting, refactoring etc. And meeting all criteria in insufficient.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit tests are conducted to check the robustness of the delivered code with a test coverage of  at least 80%. And meeting all criteria in sufficient. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Industry-standard tools are used to document the code (e.g., sphinx). And meeting all criteria in good. </t>
   </si>
   <si>
     <t>PROJECT TOTAL</t>
@@ -849,19 +840,13 @@
   </si>
   <si>
     <t>OOP</t>
-  </si>
-  <si>
-    <t>2022-23D FGA1.P1-ADSAI</t>
-  </si>
-  <si>
-    <t>Municipality of Breda</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="29">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -984,6 +969,12 @@
       <family val="2"/>
     </font>
     <font>
+      <i/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
@@ -1032,18 +1023,6 @@
     <font>
       <sz val="10"/>
       <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="16"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1838,10 +1817,10 @@
     <xf numFmtId="0" fontId="19" fillId="23" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="48" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="48" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="48" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="48" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="23" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1857,13 +1836,13 @@
     <xf numFmtId="0" fontId="19" fillId="23" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="1" applyBorder="1"/>
@@ -1896,16 +1875,16 @@
     <xf numFmtId="0" fontId="19" fillId="49" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="50" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="50" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="50" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="51" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="52" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="52" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="51" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1920,14 +1899,14 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1939,7 +1918,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1960,7 +1939,7 @@
     <xf numFmtId="0" fontId="11" fillId="54" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="52" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="52" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1981,13 +1960,13 @@
     <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="52" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="52" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="55" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="55" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="55" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="55" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2014,7 +1993,7 @@
     <xf numFmtId="0" fontId="19" fillId="56" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="55" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="55" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="56" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2026,26 +2005,21 @@
     <xf numFmtId="0" fontId="4" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -2064,8 +2038,7 @@
     <xf numFmtId="0" fontId="4" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2080,7 +2053,7 @@
     <xf numFmtId="0" fontId="4" fillId="53" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2101,13 +2074,14 @@
     <xf numFmtId="0" fontId="18" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2138,56 +2112,55 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2199,56 +2172,48 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{9902F182-0AFB-1F41-B571-EB1D4AC04E32}"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="53">
+  <dxfs count="34">
     <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFCE5CD"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
+          <fgColor rgb="FF63D297"/>
+          <bgColor rgb="FF63D297"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
       <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2439,132 +2404,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFCE5CD"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE5CD"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF63D297"/>
-          <bgColor rgb="FF63D297"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFF3F3F3"/>
           <bgColor rgb="FFF3F3F3"/>
         </patternFill>
@@ -2613,14 +2452,14 @@
   </dxfs>
   <tableStyles count="2">
     <tableStyle name="Student Self-Assessment Sheet-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="52"/>
-      <tableStyleElement type="firstRowStripe" dxfId="51"/>
-      <tableStyleElement type="secondRowStripe" dxfId="50"/>
+      <tableStyleElement type="headerRow" dxfId="33"/>
+      <tableStyleElement type="firstRowStripe" dxfId="32"/>
+      <tableStyleElement type="secondRowStripe" dxfId="31"/>
     </tableStyle>
     <tableStyle name="Copy of Student Self-Assessment-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="headerRow" dxfId="49"/>
-      <tableStyleElement type="firstRowStripe" dxfId="48"/>
-      <tableStyleElement type="secondRowStripe" dxfId="47"/>
+      <tableStyleElement type="headerRow" dxfId="30"/>
+      <tableStyleElement type="firstRowStripe" dxfId="29"/>
+      <tableStyleElement type="secondRowStripe" dxfId="28"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -2838,12 +2677,12 @@
   </sheetPr>
   <dimension ref="A1:P56"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4:I8"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="10" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D29" sqref="D29:E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3.42578125" style="39" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" style="39" customWidth="1"/>
@@ -2861,7 +2700,7 @@
     <col min="17" max="16384" width="14.42578125" style="39"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="12.95" customHeight="1">
       <c r="A1" s="17"/>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -2879,14 +2718,14 @@
       <c r="O1" s="17"/>
       <c r="P1" s="17"/>
     </row>
-    <row r="2" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" ht="23.45">
       <c r="A2" s="17"/>
       <c r="B2" s="18"/>
-      <c r="C2" s="155" t="s">
+      <c r="C2" s="202" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="156"/>
-      <c r="E2" s="156"/>
+      <c r="D2" s="203"/>
+      <c r="E2" s="203"/>
       <c r="F2" s="18"/>
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
@@ -2899,11 +2738,11 @@
       <c r="O2" s="18"/>
       <c r="P2" s="17"/>
     </row>
-    <row r="3" spans="1:16" s="23" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" s="23" customFormat="1" ht="14.45" customHeight="1">
       <c r="A3" s="19"/>
       <c r="B3" s="20"/>
-      <c r="C3" s="175"/>
-      <c r="D3" s="176"/>
+      <c r="C3" s="169"/>
+      <c r="D3" s="204"/>
       <c r="E3" s="38" t="s">
         <v>1</v>
       </c>
@@ -2913,135 +2752,135 @@
       <c r="G3" s="21"/>
       <c r="H3" s="22"/>
       <c r="I3" s="22"/>
-      <c r="J3" s="158" t="s">
+      <c r="J3" s="153" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="177"/>
-      <c r="L3" s="178" t="s">
+      <c r="K3" s="205"/>
+      <c r="L3" s="170" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="156"/>
-      <c r="N3" s="156"/>
+      <c r="M3" s="203"/>
+      <c r="N3" s="203"/>
       <c r="O3" s="20"/>
       <c r="P3" s="19"/>
     </row>
-    <row r="4" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="12.95" customHeight="1">
       <c r="A4" s="17"/>
       <c r="B4" s="24"/>
-      <c r="C4" s="179" t="s">
+      <c r="C4" s="171" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="156"/>
+      <c r="D4" s="203"/>
       <c r="E4" s="15"/>
-      <c r="F4" s="210" t="s">
-        <v>244</v>
-      </c>
-      <c r="G4" s="180"/>
-      <c r="H4" s="180"/>
-      <c r="I4" s="180"/>
-      <c r="J4" s="181"/>
-      <c r="K4" s="182"/>
-      <c r="L4" s="183" t="s">
+      <c r="F4" s="172" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="184">
+      <c r="G4" s="173"/>
+      <c r="H4" s="173"/>
+      <c r="I4" s="173"/>
+      <c r="J4" s="174"/>
+      <c r="K4" s="175"/>
+      <c r="L4" s="176" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="177">
         <f>IF(ROUND((N29/10),1)&lt;&gt;ROUND((N29/10),0),ROUND((N29/10),1),ROUND((N29/10),0))</f>
         <v>0</v>
       </c>
-      <c r="N4" s="185" t="str">
+      <c r="N4" s="178" t="str">
         <f>IF(M4&gt;=5.5,"PASS",IF(M4&gt;0,"FAIL","M/O"))</f>
         <v>M/O</v>
       </c>
       <c r="O4" s="18"/>
       <c r="P4" s="17"/>
     </row>
-    <row r="5" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="12.95" customHeight="1">
       <c r="A5" s="17"/>
       <c r="B5" s="24"/>
-      <c r="C5" s="179" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="177"/>
+      <c r="C5" s="171" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="205"/>
       <c r="E5" s="15"/>
-      <c r="F5" s="180"/>
-      <c r="G5" s="180"/>
-      <c r="H5" s="180"/>
-      <c r="I5" s="180"/>
-      <c r="J5" s="182"/>
-      <c r="K5" s="182"/>
-      <c r="L5" s="177"/>
-      <c r="M5" s="177"/>
-      <c r="N5" s="177"/>
+      <c r="F5" s="173"/>
+      <c r="G5" s="173"/>
+      <c r="H5" s="173"/>
+      <c r="I5" s="173"/>
+      <c r="J5" s="175"/>
+      <c r="K5" s="175"/>
+      <c r="L5" s="205"/>
+      <c r="M5" s="205"/>
+      <c r="N5" s="205"/>
       <c r="O5" s="18"/>
       <c r="P5" s="17"/>
     </row>
-    <row r="6" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" ht="13.9">
       <c r="A6" s="17"/>
       <c r="B6" s="24"/>
-      <c r="C6" s="179" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="186"/>
+      <c r="C6" s="171" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="179"/>
       <c r="E6" s="25" t="s">
-        <v>243</v>
-      </c>
-      <c r="F6" s="180"/>
-      <c r="G6" s="180"/>
-      <c r="H6" s="180"/>
-      <c r="I6" s="180"/>
-      <c r="J6" s="182"/>
-      <c r="K6" s="182"/>
-      <c r="L6" s="177"/>
-      <c r="M6" s="177"/>
-      <c r="N6" s="177"/>
+        <v>10</v>
+      </c>
+      <c r="F6" s="173"/>
+      <c r="G6" s="173"/>
+      <c r="H6" s="173"/>
+      <c r="I6" s="173"/>
+      <c r="J6" s="175"/>
+      <c r="K6" s="175"/>
+      <c r="L6" s="205"/>
+      <c r="M6" s="205"/>
+      <c r="N6" s="205"/>
       <c r="O6" s="18"/>
       <c r="P6" s="17"/>
     </row>
-    <row r="7" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="13.9">
       <c r="A7" s="17"/>
       <c r="B7" s="24"/>
-      <c r="C7" s="179" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="177"/>
+      <c r="C7" s="171" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="205"/>
       <c r="E7" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="180"/>
-      <c r="G7" s="180"/>
-      <c r="H7" s="180"/>
-      <c r="I7" s="180"/>
-      <c r="J7" s="182"/>
-      <c r="K7" s="182"/>
-      <c r="L7" s="177"/>
-      <c r="M7" s="177"/>
-      <c r="N7" s="177"/>
+        <v>12</v>
+      </c>
+      <c r="F7" s="173"/>
+      <c r="G7" s="173"/>
+      <c r="H7" s="173"/>
+      <c r="I7" s="173"/>
+      <c r="J7" s="175"/>
+      <c r="K7" s="175"/>
+      <c r="L7" s="205"/>
+      <c r="M7" s="205"/>
+      <c r="N7" s="205"/>
       <c r="O7" s="18"/>
       <c r="P7" s="17"/>
     </row>
-    <row r="8" spans="1:16" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="28.35" customHeight="1">
       <c r="A8" s="17"/>
       <c r="B8" s="24"/>
-      <c r="C8" s="187" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="188"/>
+      <c r="C8" s="180" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="181"/>
       <c r="E8" s="131" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="180"/>
-      <c r="G8" s="180"/>
-      <c r="H8" s="180"/>
-      <c r="I8" s="180"/>
-      <c r="J8" s="182"/>
-      <c r="K8" s="182"/>
-      <c r="L8" s="177"/>
-      <c r="M8" s="177"/>
-      <c r="N8" s="177"/>
+        <v>14</v>
+      </c>
+      <c r="F8" s="173"/>
+      <c r="G8" s="173"/>
+      <c r="H8" s="173"/>
+      <c r="I8" s="173"/>
+      <c r="J8" s="175"/>
+      <c r="K8" s="175"/>
+      <c r="L8" s="205"/>
+      <c r="M8" s="205"/>
+      <c r="N8" s="205"/>
       <c r="O8" s="18"/>
       <c r="P8" s="17"/>
     </row>
-    <row r="9" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="13.9">
       <c r="A9" s="17"/>
       <c r="B9" s="18"/>
       <c r="C9" s="18"/>
@@ -3059,7 +2898,7 @@
       <c r="O9" s="18"/>
       <c r="P9" s="17"/>
     </row>
-    <row r="10" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="13.9">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
@@ -3077,14 +2916,14 @@
       <c r="O10" s="17"/>
       <c r="P10" s="17"/>
     </row>
-    <row r="11" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" ht="23.45">
       <c r="A11" s="17"/>
       <c r="B11" s="18"/>
-      <c r="C11" s="155" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="156"/>
-      <c r="E11" s="156"/>
+      <c r="C11" s="202" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="203"/>
+      <c r="E11" s="203"/>
       <c r="F11" s="18"/>
       <c r="G11" s="18"/>
       <c r="H11" s="18"/>
@@ -3097,97 +2936,97 @@
       <c r="O11" s="18"/>
       <c r="P11" s="17"/>
     </row>
-    <row r="12" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" ht="13.9">
       <c r="A12" s="17"/>
       <c r="B12" s="18"/>
       <c r="C12" s="42"/>
       <c r="D12" s="43" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E12" s="44"/>
       <c r="F12" s="42" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G12" s="42" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H12" s="42" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I12" s="42" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J12" s="42" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="K12" s="42" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="L12" s="42" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="M12" s="42" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="N12" s="42" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="O12" s="26"/>
       <c r="P12" s="17"/>
     </row>
-    <row r="13" spans="1:16" ht="48.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" ht="48.95" customHeight="1">
       <c r="A13" s="17"/>
       <c r="B13" s="27"/>
-      <c r="C13" s="167" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="191" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="169"/>
-      <c r="F13" s="169"/>
-      <c r="G13" s="169"/>
-      <c r="H13" s="169"/>
-      <c r="I13" s="169"/>
-      <c r="J13" s="169"/>
-      <c r="K13" s="169"/>
+      <c r="C13" s="161" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="184" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="163"/>
+      <c r="F13" s="163"/>
+      <c r="G13" s="163"/>
+      <c r="H13" s="163"/>
+      <c r="I13" s="163"/>
+      <c r="J13" s="163"/>
+      <c r="K13" s="163"/>
       <c r="L13" s="120"/>
       <c r="M13" s="120"/>
       <c r="N13" s="120"/>
       <c r="O13" s="28"/>
       <c r="P13" s="17"/>
     </row>
-    <row r="14" spans="1:16" ht="118.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" ht="118.9" customHeight="1">
       <c r="A14" s="17"/>
       <c r="B14" s="27"/>
-      <c r="C14" s="167"/>
-      <c r="D14" s="170" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="170"/>
+      <c r="C14" s="161"/>
+      <c r="D14" s="164" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="164"/>
       <c r="F14" s="57" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G14" s="126" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H14" s="127" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I14" s="128" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J14" s="129" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="K14" s="130" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L14" s="41">
         <v>10</v>
       </c>
       <c r="M14" s="16" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="N14" s="41">
         <f>IF(M14="MISSING",0,IF(M14="POOR",(L14*0.2),IF(M14="INSUFFICIENT",(L14*0.4),IF(M14="SUFFICIENT",(L14*0.6),IF(M14="GOOD",(L14*0.8),IF(M14="EXCELLENT",L14,"ERROR"))))))</f>
@@ -3196,37 +3035,37 @@
       <c r="O14" s="28"/>
       <c r="P14" s="17"/>
     </row>
-    <row r="15" spans="1:16" ht="105.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" ht="105.95" customHeight="1">
       <c r="A15" s="17"/>
       <c r="B15" s="27"/>
-      <c r="C15" s="167"/>
-      <c r="D15" s="170" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="170"/>
+      <c r="C15" s="161"/>
+      <c r="D15" s="164" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="164"/>
       <c r="F15" s="57" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G15" s="135" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H15" s="40" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I15" s="136" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J15" s="137" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="K15" s="138" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="L15" s="41">
         <v>10</v>
       </c>
       <c r="M15" s="16" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="N15" s="41">
         <v>0</v>
@@ -3234,37 +3073,37 @@
       <c r="O15" s="28"/>
       <c r="P15" s="17"/>
     </row>
-    <row r="16" spans="1:16" ht="116.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" ht="116.45" customHeight="1">
       <c r="A16" s="17"/>
       <c r="B16" s="27"/>
-      <c r="C16" s="167"/>
-      <c r="D16" s="170" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" s="170"/>
+      <c r="C16" s="161"/>
+      <c r="D16" s="164" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="164"/>
       <c r="F16" s="57" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G16" s="126" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H16" s="127" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I16" s="128" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J16" s="129" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="K16" s="130" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="L16" s="41">
         <v>10</v>
       </c>
       <c r="M16" s="16" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="N16" s="41">
         <f>IF(M16="MISSING",0,IF(M16="POOR",(L16*0.2),IF(M16="INSUFFICIENT",(L16*0.4),IF(M16="SUFFICIENT",(L16*0.6),IF(M16="GOOD",(L16*0.8),IF(M16="EXCELLENT",L16,"ERROR"))))))</f>
@@ -3273,37 +3112,37 @@
       <c r="O16" s="28"/>
       <c r="P16" s="17"/>
     </row>
-    <row r="17" spans="1:16" ht="118.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" ht="118.15" customHeight="1">
       <c r="A17" s="17"/>
       <c r="B17" s="18"/>
-      <c r="C17" s="167"/>
-      <c r="D17" s="170" t="s">
-        <v>45</v>
-      </c>
-      <c r="E17" s="170"/>
+      <c r="C17" s="161"/>
+      <c r="D17" s="164" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="164"/>
       <c r="F17" s="57" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G17" s="126" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H17" s="127" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="I17" s="128" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="J17" s="129" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="K17" s="130" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L17" s="41">
         <v>10</v>
       </c>
       <c r="M17" s="16" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="N17" s="41">
         <f>IF(M17="MISSING",0,IF(M17="POOR",(L17*0.2),IF(M17="INSUFFICIENT",(L17*0.4),IF(M17="SUFFICIENT",(L17*0.6),IF(M17="GOOD",(L17*0.8),IF(M17="EXCELLENT",L17,"ERROR"))))))</f>
@@ -3312,59 +3151,59 @@
       <c r="O17" s="28"/>
       <c r="P17" s="17"/>
     </row>
-    <row r="18" spans="1:16" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" ht="48.6" customHeight="1">
       <c r="A18" s="17"/>
       <c r="B18" s="27"/>
-      <c r="C18" s="166" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="191" t="s">
-        <v>52</v>
-      </c>
-      <c r="E18" s="192"/>
-      <c r="F18" s="192"/>
-      <c r="G18" s="192"/>
-      <c r="H18" s="192"/>
-      <c r="I18" s="192"/>
-      <c r="J18" s="192"/>
-      <c r="K18" s="192"/>
+      <c r="C18" s="160" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="184" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="185"/>
+      <c r="F18" s="185"/>
+      <c r="G18" s="185"/>
+      <c r="H18" s="185"/>
+      <c r="I18" s="185"/>
+      <c r="J18" s="185"/>
+      <c r="K18" s="185"/>
       <c r="L18" s="121"/>
       <c r="M18" s="121"/>
       <c r="N18" s="121"/>
       <c r="O18" s="28"/>
       <c r="P18" s="17"/>
     </row>
-    <row r="19" spans="1:16" ht="118.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" ht="118.7" customHeight="1">
       <c r="A19" s="17"/>
       <c r="B19" s="18"/>
-      <c r="C19" s="166"/>
-      <c r="D19" s="193" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" s="193"/>
+      <c r="C19" s="160"/>
+      <c r="D19" s="186" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="186"/>
       <c r="F19" s="123" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G19" s="50" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H19" s="51" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I19" s="52" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="J19" s="53" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K19" s="54" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L19" s="41">
         <v>10</v>
       </c>
       <c r="M19" s="16" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="N19" s="41">
         <f>IF(M19="MISSING",0,IF(M19="POOR",(L19*0.2),IF(M19="INSUFFICIENT",(L19*0.4),IF(M19="SUFFICIENT",(L19*0.6),IF(M19="GOOD",(L19*0.8),IF(M19="EXCELLENT",L19,"ERROR"))))))</f>
@@ -3373,59 +3212,59 @@
       <c r="O19" s="28"/>
       <c r="P19" s="17"/>
     </row>
-    <row r="20" spans="1:16" s="59" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" s="59" customFormat="1" ht="48" customHeight="1">
       <c r="A20" s="17"/>
       <c r="B20" s="27"/>
-      <c r="C20" s="166" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" s="168" t="s">
-        <v>60</v>
-      </c>
-      <c r="E20" s="169"/>
-      <c r="F20" s="169"/>
-      <c r="G20" s="169"/>
-      <c r="H20" s="169"/>
-      <c r="I20" s="169"/>
-      <c r="J20" s="169"/>
-      <c r="K20" s="169"/>
+      <c r="C20" s="160" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="162" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="163"/>
+      <c r="F20" s="163"/>
+      <c r="G20" s="163"/>
+      <c r="H20" s="163"/>
+      <c r="I20" s="163"/>
+      <c r="J20" s="163"/>
+      <c r="K20" s="163"/>
       <c r="L20" s="122"/>
       <c r="M20" s="122"/>
       <c r="N20" s="122"/>
       <c r="O20" s="28"/>
       <c r="P20" s="17"/>
     </row>
-    <row r="21" spans="1:16" s="59" customFormat="1" ht="136.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" s="59" customFormat="1" ht="136.5" customHeight="1">
       <c r="A21" s="17"/>
       <c r="B21" s="18"/>
-      <c r="C21" s="166"/>
-      <c r="D21" s="189" t="s">
-        <v>61</v>
-      </c>
-      <c r="E21" s="190"/>
+      <c r="C21" s="160"/>
+      <c r="D21" s="182" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" s="183"/>
       <c r="F21" s="57" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G21" s="50" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H21" s="51" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I21" s="52" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="J21" s="53" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K21" s="54" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L21" s="41">
         <v>10</v>
       </c>
       <c r="M21" s="124" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="N21" s="41">
         <f>IF(M21="MISSING",0,IF(M21="POOR",(L21*0.2),IF(M21="INSUFFICIENT",(L21*0.4),IF(M21="SUFFICIENT",(L21*0.6),IF(M21="GOOD",(L21*0.8),IF(M21="EXCELLENT",L21,"ERROR"))))))</f>
@@ -3434,59 +3273,59 @@
       <c r="O21" s="28"/>
       <c r="P21" s="17"/>
     </row>
-    <row r="22" spans="1:16" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" ht="48" customHeight="1">
       <c r="A22" s="17"/>
       <c r="B22" s="27"/>
-      <c r="C22" s="166" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" s="168" t="s">
-        <v>69</v>
-      </c>
-      <c r="E22" s="169"/>
-      <c r="F22" s="169"/>
-      <c r="G22" s="169"/>
-      <c r="H22" s="169"/>
-      <c r="I22" s="169"/>
-      <c r="J22" s="169"/>
-      <c r="K22" s="169"/>
+      <c r="C22" s="160" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="162" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="163"/>
+      <c r="F22" s="163"/>
+      <c r="G22" s="163"/>
+      <c r="H22" s="163"/>
+      <c r="I22" s="163"/>
+      <c r="J22" s="163"/>
+      <c r="K22" s="163"/>
       <c r="L22" s="122"/>
       <c r="M22" s="122"/>
       <c r="N22" s="122"/>
       <c r="O22" s="28"/>
       <c r="P22" s="17"/>
     </row>
-    <row r="23" spans="1:16" ht="108" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" ht="108" customHeight="1">
       <c r="A23" s="17"/>
       <c r="B23" s="18"/>
-      <c r="C23" s="166"/>
-      <c r="D23" s="170" t="s">
-        <v>70</v>
-      </c>
-      <c r="E23" s="171"/>
+      <c r="C23" s="160"/>
+      <c r="D23" s="164" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23" s="165"/>
       <c r="F23" s="139" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G23" s="140" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H23" s="127" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I23" s="128" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J23" s="129" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K23" s="130" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L23" s="41">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="M23" s="16" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="N23" s="41">
         <f>IF(M23="MISSING",0,IF(M23="POOR",(L23*0.2),IF(M23="INSUFFICIENT",(L23*0.4),IF(M23="SUFFICIENT",(L23*0.6),IF(M23="GOOD",(L23*0.8),IF(M23="EXCELLENT",L23,"ERROR"))))))</f>
@@ -3495,59 +3334,59 @@
       <c r="O23" s="28"/>
       <c r="P23" s="17"/>
     </row>
-    <row r="24" spans="1:16" ht="42.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" ht="42.95" customHeight="1">
       <c r="A24" s="17"/>
       <c r="B24" s="27"/>
-      <c r="C24" s="167" t="s">
-        <v>76</v>
-      </c>
-      <c r="D24" s="172" t="s">
-        <v>77</v>
-      </c>
-      <c r="E24" s="172"/>
-      <c r="F24" s="172"/>
-      <c r="G24" s="172"/>
-      <c r="H24" s="172"/>
-      <c r="I24" s="172"/>
-      <c r="J24" s="172"/>
-      <c r="K24" s="172"/>
+      <c r="C24" s="161" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" s="166" t="s">
+        <v>79</v>
+      </c>
+      <c r="E24" s="166"/>
+      <c r="F24" s="166"/>
+      <c r="G24" s="166"/>
+      <c r="H24" s="166"/>
+      <c r="I24" s="166"/>
+      <c r="J24" s="166"/>
+      <c r="K24" s="166"/>
       <c r="L24" s="45"/>
       <c r="M24" s="45"/>
       <c r="N24" s="45"/>
       <c r="O24" s="28"/>
       <c r="P24" s="17"/>
     </row>
-    <row r="25" spans="1:16" s="56" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" s="56" customFormat="1" ht="144" customHeight="1">
       <c r="A25" s="48"/>
       <c r="B25" s="49"/>
-      <c r="C25" s="156"/>
-      <c r="D25" s="173" t="s">
-        <v>78</v>
-      </c>
-      <c r="E25" s="173"/>
+      <c r="C25" s="203"/>
+      <c r="D25" s="167" t="s">
+        <v>80</v>
+      </c>
+      <c r="E25" s="167"/>
       <c r="F25" s="64" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G25" s="141" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="H25" s="127" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I25" s="128" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="J25" s="129" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="K25" s="130" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="L25" s="41">
         <v>10</v>
       </c>
       <c r="M25" s="16" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="N25" s="41">
         <f>IF(M25="MISSING",0,IF(M25="POOR",(L25*0.2),IF(M25="INSUFFICIENT",(L25*0.4),IF(M25="SUFFICIENT",(L25*0.6),IF(M25="GOOD",(L25*0.8),IF(M25="EXCELLENT",L25,"ERROR"))))))</f>
@@ -3556,20 +3395,20 @@
       <c r="O25" s="55"/>
       <c r="P25" s="48"/>
     </row>
-    <row r="26" spans="1:16" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" ht="53.1" customHeight="1">
       <c r="A26" s="17"/>
       <c r="B26" s="18"/>
-      <c r="C26" s="166" t="s">
-        <v>84</v>
-      </c>
-      <c r="D26" s="168" t="s">
-        <v>85</v>
-      </c>
-      <c r="E26" s="168"/>
-      <c r="F26" s="168"/>
-      <c r="G26" s="168"/>
-      <c r="H26" s="168"/>
-      <c r="I26" s="168"/>
+      <c r="C26" s="160" t="s">
+        <v>86</v>
+      </c>
+      <c r="D26" s="162" t="s">
+        <v>87</v>
+      </c>
+      <c r="E26" s="162"/>
+      <c r="F26" s="162"/>
+      <c r="G26" s="162"/>
+      <c r="H26" s="162"/>
+      <c r="I26" s="162"/>
       <c r="J26" s="113"/>
       <c r="K26" s="113"/>
       <c r="L26" s="122"/>
@@ -3578,37 +3417,37 @@
       <c r="O26" s="28"/>
       <c r="P26" s="17"/>
     </row>
-    <row r="27" spans="1:16" ht="111" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" ht="111" customHeight="1">
       <c r="A27" s="17"/>
       <c r="B27" s="18"/>
-      <c r="C27" s="166"/>
-      <c r="D27" s="170" t="s">
-        <v>86</v>
-      </c>
-      <c r="E27" s="170"/>
+      <c r="C27" s="160"/>
+      <c r="D27" s="164" t="s">
+        <v>88</v>
+      </c>
+      <c r="E27" s="164"/>
       <c r="F27" s="57" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G27" s="126" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="H27" s="127" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I27" s="128" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J27" s="129" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K27" s="130" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L27" s="41">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="M27" s="16" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="N27" s="41">
         <f>IF(M27="MISSING",0,IF(M27="POOR",(L27*0.2),IF(M27="INSUFFICIENT",(L27*0.4),IF(M27="SUFFICIENT",(L27*0.6),IF(M27="GOOD",(L27*0.8),IF(M27="EXCELLENT",L27,"ERROR"))))))</f>
@@ -3617,59 +3456,59 @@
       <c r="O27" s="28"/>
       <c r="P27" s="17"/>
     </row>
-    <row r="28" spans="1:16" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" ht="53.1" customHeight="1">
       <c r="A28" s="17"/>
       <c r="B28" s="18"/>
-      <c r="C28" s="166" t="s">
-        <v>92</v>
-      </c>
-      <c r="D28" s="174" t="s">
+      <c r="C28" s="160" t="s">
         <v>93</v>
       </c>
-      <c r="E28" s="174"/>
-      <c r="F28" s="174"/>
-      <c r="G28" s="174"/>
-      <c r="H28" s="174"/>
-      <c r="I28" s="174"/>
-      <c r="J28" s="174"/>
-      <c r="K28" s="174"/>
+      <c r="D28" s="168" t="s">
+        <v>94</v>
+      </c>
+      <c r="E28" s="168"/>
+      <c r="F28" s="168"/>
+      <c r="G28" s="168"/>
+      <c r="H28" s="168"/>
+      <c r="I28" s="168"/>
+      <c r="J28" s="168"/>
+      <c r="K28" s="168"/>
       <c r="L28" s="122"/>
       <c r="M28" s="122"/>
       <c r="N28" s="122"/>
       <c r="O28" s="28"/>
       <c r="P28" s="17"/>
     </row>
-    <row r="29" spans="1:16" s="63" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" s="63" customFormat="1" ht="150" customHeight="1">
       <c r="A29" s="60"/>
       <c r="B29" s="61"/>
-      <c r="C29" s="166"/>
-      <c r="D29" s="170" t="s">
-        <v>94</v>
-      </c>
-      <c r="E29" s="170"/>
+      <c r="C29" s="160"/>
+      <c r="D29" s="164" t="s">
+        <v>95</v>
+      </c>
+      <c r="E29" s="164"/>
       <c r="F29" s="57" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G29" s="126" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H29" s="127" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I29" s="128" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="J29" s="129" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="K29" s="130" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="L29" s="41">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="M29" s="16" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="N29" s="41">
         <f>IF(M29="MISSING",0,IF(M29="POOR",(L29*0.2),IF(M29="INSUFFICIENT",(L29*0.4),IF(M29="SUFFICIENT",(L29*0.6),IF(M29="GOOD",(L29*0.8),IF(M29="EXCELLENT",L29,"ERROR"))))))</f>
@@ -3678,7 +3517,7 @@
       <c r="O29" s="62"/>
       <c r="P29" s="60"/>
     </row>
-    <row r="30" spans="1:16" ht="35.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" ht="35.85" customHeight="1">
       <c r="A30" s="17"/>
       <c r="B30" s="27"/>
       <c r="C30" s="18"/>
@@ -3688,7 +3527,7 @@
       <c r="G30" s="18"/>
       <c r="H30" s="18"/>
       <c r="I30" s="58" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J30" s="58"/>
       <c r="K30" s="58"/>
@@ -3697,7 +3536,7 @@
         <v>100</v>
       </c>
       <c r="M30" s="47" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="N30" s="41">
         <f>SUM(N14:N29)</f>
@@ -3706,7 +3545,7 @@
       <c r="O30" s="28"/>
       <c r="P30" s="17"/>
     </row>
-    <row r="31" spans="1:16" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" ht="17.45" customHeight="1">
       <c r="A31" s="17"/>
       <c r="B31" s="18"/>
       <c r="C31" s="18"/>
@@ -3724,7 +3563,7 @@
       <c r="O31" s="28"/>
       <c r="P31" s="17"/>
     </row>
-    <row r="32" spans="1:16" s="59" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" s="59" customFormat="1" ht="13.9">
       <c r="A32" s="17"/>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
@@ -3742,14 +3581,14 @@
       <c r="O32" s="17"/>
       <c r="P32" s="17"/>
     </row>
-    <row r="33" spans="1:16" s="59" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:16" s="59" customFormat="1" ht="23.45">
       <c r="A33" s="17"/>
       <c r="B33" s="29"/>
-      <c r="C33" s="155" t="s">
-        <v>102</v>
-      </c>
-      <c r="D33" s="156"/>
-      <c r="E33" s="156"/>
+      <c r="C33" s="202" t="s">
+        <v>103</v>
+      </c>
+      <c r="D33" s="203"/>
+      <c r="E33" s="203"/>
       <c r="F33" s="29"/>
       <c r="G33" s="29"/>
       <c r="H33" s="29"/>
@@ -3762,343 +3601,343 @@
       <c r="O33" s="30"/>
       <c r="P33" s="17"/>
     </row>
-    <row r="34" spans="1:16" s="59" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" s="59" customFormat="1" ht="13.9">
       <c r="A34" s="17"/>
       <c r="B34" s="29"/>
       <c r="C34" s="109" t="s">
-        <v>103</v>
-      </c>
-      <c r="D34" s="158" t="s">
         <v>104</v>
       </c>
-      <c r="E34" s="156"/>
+      <c r="D34" s="153" t="s">
+        <v>105</v>
+      </c>
+      <c r="E34" s="203"/>
       <c r="F34" s="109" t="s">
-        <v>105</v>
-      </c>
-      <c r="G34" s="158" t="s">
+        <v>106</v>
+      </c>
+      <c r="G34" s="153" t="s">
         <v>2</v>
       </c>
-      <c r="H34" s="156"/>
-      <c r="I34" s="156"/>
-      <c r="J34" s="156"/>
-      <c r="K34" s="156"/>
+      <c r="H34" s="203"/>
+      <c r="I34" s="203"/>
+      <c r="J34" s="203"/>
+      <c r="K34" s="203"/>
       <c r="L34" s="65"/>
       <c r="M34" s="109"/>
       <c r="N34" s="110" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="O34" s="29"/>
       <c r="P34" s="17"/>
     </row>
-    <row r="35" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A35" s="17"/>
       <c r="B35" s="29"/>
       <c r="C35" s="66">
         <v>9</v>
       </c>
-      <c r="D35" s="165" t="s">
-        <v>107</v>
-      </c>
-      <c r="E35" s="163"/>
+      <c r="D35" s="159" t="s">
+        <v>108</v>
+      </c>
+      <c r="E35" s="206"/>
       <c r="F35" s="111" t="s">
-        <v>108</v>
-      </c>
-      <c r="G35" s="164" t="s">
         <v>109</v>
       </c>
-      <c r="H35" s="164"/>
-      <c r="I35" s="164"/>
-      <c r="J35" s="164"/>
-      <c r="K35" s="164"/>
-      <c r="L35" s="164"/>
-      <c r="M35" s="164"/>
+      <c r="G35" s="158" t="s">
+        <v>110</v>
+      </c>
+      <c r="H35" s="158"/>
+      <c r="I35" s="158"/>
+      <c r="J35" s="158"/>
+      <c r="K35" s="158"/>
+      <c r="L35" s="158"/>
+      <c r="M35" s="158"/>
       <c r="N35" s="67">
         <v>3</v>
       </c>
       <c r="O35" s="29"/>
       <c r="P35" s="17"/>
     </row>
-    <row r="36" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A36" s="17"/>
       <c r="B36" s="29"/>
       <c r="C36" s="68">
         <v>10</v>
       </c>
-      <c r="D36" s="162" t="s">
-        <v>107</v>
-      </c>
-      <c r="E36" s="163"/>
+      <c r="D36" s="157" t="s">
+        <v>108</v>
+      </c>
+      <c r="E36" s="206"/>
       <c r="F36" s="111" t="s">
-        <v>110</v>
-      </c>
-      <c r="G36" s="164" t="s">
         <v>111</v>
       </c>
-      <c r="H36" s="164"/>
-      <c r="I36" s="164"/>
-      <c r="J36" s="164"/>
-      <c r="K36" s="164"/>
-      <c r="L36" s="164"/>
-      <c r="M36" s="164"/>
+      <c r="G36" s="158" t="s">
+        <v>112</v>
+      </c>
+      <c r="H36" s="158"/>
+      <c r="I36" s="158"/>
+      <c r="J36" s="158"/>
+      <c r="K36" s="158"/>
+      <c r="L36" s="158"/>
+      <c r="M36" s="158"/>
       <c r="N36" s="69">
         <v>3</v>
       </c>
       <c r="O36" s="29"/>
       <c r="P36" s="17"/>
     </row>
-    <row r="37" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A37" s="17"/>
       <c r="B37" s="29"/>
       <c r="C37" s="66">
         <v>11</v>
       </c>
-      <c r="D37" s="165" t="s">
-        <v>107</v>
-      </c>
-      <c r="E37" s="163"/>
+      <c r="D37" s="159" t="s">
+        <v>108</v>
+      </c>
+      <c r="E37" s="206"/>
       <c r="F37" s="111" t="s">
-        <v>112</v>
-      </c>
-      <c r="G37" s="164" t="s">
         <v>113</v>
       </c>
-      <c r="H37" s="164"/>
-      <c r="I37" s="164"/>
-      <c r="J37" s="164"/>
-      <c r="K37" s="164"/>
-      <c r="L37" s="164"/>
-      <c r="M37" s="164"/>
+      <c r="G37" s="158" t="s">
+        <v>114</v>
+      </c>
+      <c r="H37" s="158"/>
+      <c r="I37" s="158"/>
+      <c r="J37" s="158"/>
+      <c r="K37" s="158"/>
+      <c r="L37" s="158"/>
+      <c r="M37" s="158"/>
       <c r="N37" s="67">
         <v>3</v>
       </c>
       <c r="O37" s="29"/>
       <c r="P37" s="17"/>
     </row>
-    <row r="38" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A38" s="17"/>
       <c r="B38" s="29"/>
       <c r="C38" s="70">
         <v>1</v>
       </c>
       <c r="D38" s="146" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E38" s="146"/>
       <c r="F38" s="112" t="s">
-        <v>115</v>
-      </c>
-      <c r="G38" s="148" t="s">
         <v>116</v>
       </c>
-      <c r="H38" s="148"/>
-      <c r="I38" s="148"/>
-      <c r="J38" s="148"/>
-      <c r="K38" s="148"/>
-      <c r="L38" s="148"/>
-      <c r="M38" s="148"/>
+      <c r="G38" s="147" t="s">
+        <v>117</v>
+      </c>
+      <c r="H38" s="147"/>
+      <c r="I38" s="147"/>
+      <c r="J38" s="147"/>
+      <c r="K38" s="147"/>
+      <c r="L38" s="147"/>
+      <c r="M38" s="147"/>
       <c r="N38" s="71">
         <v>3</v>
       </c>
       <c r="O38" s="29"/>
       <c r="P38" s="17"/>
     </row>
-    <row r="39" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A39" s="17"/>
       <c r="B39" s="29"/>
       <c r="C39" s="72">
         <v>2</v>
       </c>
-      <c r="D39" s="149" t="s">
-        <v>114</v>
-      </c>
-      <c r="E39" s="150"/>
+      <c r="D39" s="148" t="s">
+        <v>115</v>
+      </c>
+      <c r="E39" s="207"/>
       <c r="F39" s="114" t="s">
-        <v>117</v>
-      </c>
-      <c r="G39" s="151" t="s">
         <v>118</v>
       </c>
-      <c r="H39" s="151"/>
-      <c r="I39" s="151"/>
-      <c r="J39" s="151"/>
-      <c r="K39" s="151"/>
-      <c r="L39" s="151"/>
-      <c r="M39" s="151"/>
+      <c r="G39" s="149" t="s">
+        <v>119</v>
+      </c>
+      <c r="H39" s="149"/>
+      <c r="I39" s="149"/>
+      <c r="J39" s="149"/>
+      <c r="K39" s="149"/>
+      <c r="L39" s="149"/>
+      <c r="M39" s="149"/>
       <c r="N39" s="73">
         <v>3</v>
       </c>
       <c r="O39" s="29"/>
       <c r="P39" s="17"/>
     </row>
-    <row r="40" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A40" s="17"/>
       <c r="B40" s="29"/>
       <c r="C40" s="74">
         <v>3</v>
       </c>
-      <c r="D40" s="152" t="s">
-        <v>119</v>
-      </c>
-      <c r="E40" s="153"/>
+      <c r="D40" s="150" t="s">
+        <v>120</v>
+      </c>
+      <c r="E40" s="208"/>
       <c r="F40" s="112" t="s">
-        <v>120</v>
-      </c>
-      <c r="G40" s="148" t="s">
         <v>121</v>
       </c>
-      <c r="H40" s="148"/>
-      <c r="I40" s="148"/>
-      <c r="J40" s="148"/>
-      <c r="K40" s="148"/>
-      <c r="L40" s="148"/>
-      <c r="M40" s="148"/>
+      <c r="G40" s="147" t="s">
+        <v>122</v>
+      </c>
+      <c r="H40" s="147"/>
+      <c r="I40" s="147"/>
+      <c r="J40" s="147"/>
+      <c r="K40" s="147"/>
+      <c r="L40" s="147"/>
+      <c r="M40" s="147"/>
       <c r="N40" s="75">
         <v>3</v>
       </c>
       <c r="O40" s="29"/>
       <c r="P40" s="17"/>
     </row>
-    <row r="41" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A41" s="17"/>
       <c r="B41" s="29"/>
       <c r="C41" s="76">
         <v>4</v>
       </c>
-      <c r="D41" s="154" t="s">
-        <v>122</v>
-      </c>
-      <c r="E41" s="150"/>
+      <c r="D41" s="151" t="s">
+        <v>123</v>
+      </c>
+      <c r="E41" s="207"/>
       <c r="F41" s="114" t="s">
-        <v>123</v>
-      </c>
-      <c r="G41" s="151" t="s">
         <v>124</v>
       </c>
-      <c r="H41" s="151"/>
-      <c r="I41" s="151"/>
-      <c r="J41" s="151"/>
-      <c r="K41" s="151"/>
-      <c r="L41" s="151"/>
-      <c r="M41" s="151"/>
+      <c r="G41" s="149" t="s">
+        <v>125</v>
+      </c>
+      <c r="H41" s="149"/>
+      <c r="I41" s="149"/>
+      <c r="J41" s="149"/>
+      <c r="K41" s="149"/>
+      <c r="L41" s="149"/>
+      <c r="M41" s="149"/>
       <c r="N41" s="77">
         <v>3</v>
       </c>
       <c r="O41" s="29"/>
       <c r="P41" s="17"/>
     </row>
-    <row r="42" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A42" s="17"/>
       <c r="B42" s="29"/>
       <c r="C42" s="70">
         <v>5</v>
       </c>
       <c r="D42" s="146" t="s">
-        <v>125</v>
-      </c>
-      <c r="E42" s="147"/>
+        <v>126</v>
+      </c>
+      <c r="E42" s="209"/>
       <c r="F42" s="112" t="s">
-        <v>125</v>
-      </c>
-      <c r="G42" s="148" t="s">
         <v>126</v>
       </c>
-      <c r="H42" s="148"/>
-      <c r="I42" s="148"/>
-      <c r="J42" s="148"/>
-      <c r="K42" s="148"/>
-      <c r="L42" s="148"/>
-      <c r="M42" s="148"/>
+      <c r="G42" s="147" t="s">
+        <v>127</v>
+      </c>
+      <c r="H42" s="147"/>
+      <c r="I42" s="147"/>
+      <c r="J42" s="147"/>
+      <c r="K42" s="147"/>
+      <c r="L42" s="147"/>
+      <c r="M42" s="147"/>
       <c r="N42" s="71">
         <v>3</v>
       </c>
       <c r="O42" s="29"/>
       <c r="P42" s="17"/>
     </row>
-    <row r="43" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A43" s="17"/>
       <c r="B43" s="29"/>
       <c r="C43" s="72">
         <v>6</v>
       </c>
-      <c r="D43" s="149" t="s">
-        <v>125</v>
-      </c>
-      <c r="E43" s="150"/>
+      <c r="D43" s="148" t="s">
+        <v>126</v>
+      </c>
+      <c r="E43" s="207"/>
       <c r="F43" s="114" t="s">
-        <v>127</v>
-      </c>
-      <c r="G43" s="151" t="s">
         <v>128</v>
       </c>
-      <c r="H43" s="151"/>
-      <c r="I43" s="151"/>
-      <c r="J43" s="151"/>
-      <c r="K43" s="151"/>
-      <c r="L43" s="151"/>
-      <c r="M43" s="151"/>
+      <c r="G43" s="149" t="s">
+        <v>129</v>
+      </c>
+      <c r="H43" s="149"/>
+      <c r="I43" s="149"/>
+      <c r="J43" s="149"/>
+      <c r="K43" s="149"/>
+      <c r="L43" s="149"/>
+      <c r="M43" s="149"/>
       <c r="N43" s="73">
         <v>3</v>
       </c>
       <c r="O43" s="29"/>
       <c r="P43" s="17"/>
     </row>
-    <row r="44" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A44" s="17"/>
       <c r="B44" s="29"/>
       <c r="C44" s="74">
         <v>7</v>
       </c>
-      <c r="D44" s="152" t="s">
-        <v>129</v>
-      </c>
-      <c r="E44" s="153"/>
+      <c r="D44" s="150" t="s">
+        <v>130</v>
+      </c>
+      <c r="E44" s="208"/>
       <c r="F44" s="112" t="s">
-        <v>130</v>
-      </c>
-      <c r="G44" s="148" t="s">
         <v>131</v>
       </c>
-      <c r="H44" s="148"/>
-      <c r="I44" s="148"/>
-      <c r="J44" s="148"/>
-      <c r="K44" s="148"/>
-      <c r="L44" s="148"/>
-      <c r="M44" s="148"/>
+      <c r="G44" s="147" t="s">
+        <v>132</v>
+      </c>
+      <c r="H44" s="147"/>
+      <c r="I44" s="147"/>
+      <c r="J44" s="147"/>
+      <c r="K44" s="147"/>
+      <c r="L44" s="147"/>
+      <c r="M44" s="147"/>
       <c r="N44" s="75">
         <v>3</v>
       </c>
       <c r="O44" s="29"/>
       <c r="P44" s="17"/>
     </row>
-    <row r="45" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A45" s="17"/>
       <c r="B45" s="29"/>
       <c r="C45" s="76">
         <v>8</v>
       </c>
-      <c r="D45" s="154" t="s">
-        <v>129</v>
-      </c>
-      <c r="E45" s="150"/>
+      <c r="D45" s="151" t="s">
+        <v>130</v>
+      </c>
+      <c r="E45" s="207"/>
       <c r="F45" s="114" t="s">
-        <v>132</v>
-      </c>
-      <c r="G45" s="151" t="s">
         <v>133</v>
       </c>
-      <c r="H45" s="151"/>
-      <c r="I45" s="151"/>
-      <c r="J45" s="151"/>
-      <c r="K45" s="151"/>
-      <c r="L45" s="151"/>
-      <c r="M45" s="151"/>
+      <c r="G45" s="149" t="s">
+        <v>134</v>
+      </c>
+      <c r="H45" s="149"/>
+      <c r="I45" s="149"/>
+      <c r="J45" s="149"/>
+      <c r="K45" s="149"/>
+      <c r="L45" s="149"/>
+      <c r="M45" s="149"/>
       <c r="N45" s="77">
         <v>3</v>
       </c>
       <c r="O45" s="29"/>
       <c r="P45" s="17"/>
     </row>
-    <row r="46" spans="1:16" s="59" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" s="59" customFormat="1" ht="13.9">
       <c r="A46" s="17"/>
       <c r="B46" s="29"/>
       <c r="C46" s="29"/>
@@ -4116,7 +3955,7 @@
       <c r="O46" s="29"/>
       <c r="P46" s="17"/>
     </row>
-    <row r="47" spans="1:16" s="59" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" s="59" customFormat="1" ht="13.9">
       <c r="A47" s="17"/>
       <c r="B47" s="17"/>
       <c r="C47" s="17"/>
@@ -4134,14 +3973,14 @@
       <c r="O47" s="17"/>
       <c r="P47" s="17"/>
     </row>
-    <row r="48" spans="1:16" s="59" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:16" s="59" customFormat="1" ht="23.45">
       <c r="A48" s="17"/>
       <c r="B48" s="32"/>
-      <c r="C48" s="155" t="s">
-        <v>134</v>
-      </c>
-      <c r="D48" s="156"/>
-      <c r="E48" s="156"/>
+      <c r="C48" s="202" t="s">
+        <v>135</v>
+      </c>
+      <c r="D48" s="203"/>
+      <c r="E48" s="203"/>
       <c r="F48" s="27"/>
       <c r="G48" s="18"/>
       <c r="H48" s="18"/>
@@ -4154,163 +3993,163 @@
       <c r="O48" s="18"/>
       <c r="P48" s="17"/>
     </row>
-    <row r="49" spans="1:16" s="59" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" s="59" customFormat="1" ht="13.9">
       <c r="A49" s="17"/>
       <c r="B49" s="32"/>
       <c r="C49" s="33" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D49" s="33" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E49" s="115"/>
-      <c r="F49" s="157" t="s">
-        <v>136</v>
-      </c>
-      <c r="G49" s="156"/>
-      <c r="H49" s="156"/>
-      <c r="I49" s="156"/>
-      <c r="J49" s="158" t="s">
+      <c r="F49" s="152" t="s">
         <v>137</v>
       </c>
-      <c r="K49" s="156"/>
-      <c r="L49" s="156"/>
-      <c r="M49" s="156"/>
-      <c r="N49" s="156"/>
+      <c r="G49" s="203"/>
+      <c r="H49" s="203"/>
+      <c r="I49" s="203"/>
+      <c r="J49" s="153" t="s">
+        <v>138</v>
+      </c>
+      <c r="K49" s="203"/>
+      <c r="L49" s="203"/>
+      <c r="M49" s="203"/>
+      <c r="N49" s="203"/>
       <c r="O49" s="18"/>
       <c r="P49" s="17"/>
     </row>
-    <row r="50" spans="1:16" s="59" customFormat="1" ht="49.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" s="59" customFormat="1" ht="49.35" customHeight="1">
       <c r="A50" s="17"/>
       <c r="B50" s="34"/>
       <c r="C50" s="35">
         <v>1</v>
       </c>
       <c r="D50" s="36" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E50" s="117"/>
-      <c r="F50" s="159" t="s">
-        <v>139</v>
-      </c>
-      <c r="G50" s="160"/>
-      <c r="H50" s="160"/>
-      <c r="I50" s="160"/>
-      <c r="J50" s="159" t="s">
+      <c r="F50" s="154" t="s">
         <v>140</v>
       </c>
-      <c r="K50" s="160"/>
-      <c r="L50" s="160"/>
-      <c r="M50" s="160"/>
-      <c r="N50" s="160"/>
+      <c r="G50" s="155"/>
+      <c r="H50" s="155"/>
+      <c r="I50" s="155"/>
+      <c r="J50" s="154" t="s">
+        <v>141</v>
+      </c>
+      <c r="K50" s="155"/>
+      <c r="L50" s="155"/>
+      <c r="M50" s="155"/>
+      <c r="N50" s="155"/>
       <c r="O50" s="18"/>
       <c r="P50" s="17"/>
     </row>
-    <row r="51" spans="1:16" s="59" customFormat="1" ht="47.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" s="59" customFormat="1" ht="47.45" customHeight="1">
       <c r="A51" s="17"/>
       <c r="B51" s="34"/>
       <c r="C51" s="37">
         <v>2</v>
       </c>
       <c r="D51" s="31" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E51" s="116"/>
-      <c r="F51" s="161" t="s">
-        <v>142</v>
-      </c>
-      <c r="G51" s="160"/>
-      <c r="H51" s="160"/>
-      <c r="I51" s="160"/>
-      <c r="J51" s="161" t="s">
+      <c r="F51" s="156" t="s">
         <v>143</v>
       </c>
-      <c r="K51" s="160"/>
-      <c r="L51" s="160"/>
-      <c r="M51" s="160"/>
-      <c r="N51" s="160"/>
+      <c r="G51" s="155"/>
+      <c r="H51" s="155"/>
+      <c r="I51" s="155"/>
+      <c r="J51" s="156" t="s">
+        <v>144</v>
+      </c>
+      <c r="K51" s="155"/>
+      <c r="L51" s="155"/>
+      <c r="M51" s="155"/>
+      <c r="N51" s="155"/>
       <c r="O51" s="18"/>
       <c r="P51" s="17"/>
     </row>
-    <row r="52" spans="1:16" s="59" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" s="59" customFormat="1" ht="42" customHeight="1">
       <c r="A52" s="17"/>
       <c r="B52" s="34"/>
       <c r="C52" s="35">
         <v>3</v>
       </c>
       <c r="D52" s="36" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E52" s="117"/>
-      <c r="F52" s="159" t="s">
-        <v>145</v>
-      </c>
-      <c r="G52" s="160"/>
-      <c r="H52" s="160"/>
-      <c r="I52" s="160"/>
-      <c r="J52" s="159" t="s">
+      <c r="F52" s="154" t="s">
         <v>146</v>
       </c>
-      <c r="K52" s="160"/>
-      <c r="L52" s="160"/>
-      <c r="M52" s="160"/>
-      <c r="N52" s="160"/>
+      <c r="G52" s="155"/>
+      <c r="H52" s="155"/>
+      <c r="I52" s="155"/>
+      <c r="J52" s="154" t="s">
+        <v>147</v>
+      </c>
+      <c r="K52" s="155"/>
+      <c r="L52" s="155"/>
+      <c r="M52" s="155"/>
+      <c r="N52" s="155"/>
       <c r="O52" s="18"/>
       <c r="P52" s="17"/>
     </row>
-    <row r="53" spans="1:16" s="59" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" s="59" customFormat="1" ht="42.6" customHeight="1">
       <c r="A53" s="17"/>
       <c r="B53" s="34"/>
       <c r="C53" s="37">
         <v>4</v>
       </c>
       <c r="D53" s="31" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E53" s="116"/>
-      <c r="F53" s="161" t="s">
-        <v>148</v>
-      </c>
-      <c r="G53" s="160"/>
-      <c r="H53" s="160"/>
-      <c r="I53" s="160"/>
-      <c r="J53" s="161" t="s">
+      <c r="F53" s="156" t="s">
         <v>149</v>
       </c>
-      <c r="K53" s="160"/>
-      <c r="L53" s="160"/>
-      <c r="M53" s="160"/>
-      <c r="N53" s="160"/>
+      <c r="G53" s="155"/>
+      <c r="H53" s="155"/>
+      <c r="I53" s="155"/>
+      <c r="J53" s="156" t="s">
+        <v>150</v>
+      </c>
+      <c r="K53" s="155"/>
+      <c r="L53" s="155"/>
+      <c r="M53" s="155"/>
+      <c r="N53" s="155"/>
       <c r="O53" s="18"/>
       <c r="P53" s="17"/>
     </row>
-    <row r="54" spans="1:16" s="59" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" s="59" customFormat="1" ht="36" customHeight="1">
       <c r="A54" s="17"/>
       <c r="B54" s="34"/>
       <c r="C54" s="35">
         <v>5</v>
       </c>
       <c r="D54" s="36" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E54" s="117"/>
-      <c r="F54" s="159" t="s">
-        <v>151</v>
-      </c>
-      <c r="G54" s="160"/>
-      <c r="H54" s="160"/>
-      <c r="I54" s="160"/>
-      <c r="J54" s="159" t="s">
+      <c r="F54" s="154" t="s">
         <v>152</v>
       </c>
-      <c r="K54" s="160"/>
-      <c r="L54" s="160"/>
-      <c r="M54" s="160"/>
-      <c r="N54" s="160"/>
+      <c r="G54" s="155"/>
+      <c r="H54" s="155"/>
+      <c r="I54" s="155"/>
+      <c r="J54" s="154" t="s">
+        <v>153</v>
+      </c>
+      <c r="K54" s="155"/>
+      <c r="L54" s="155"/>
+      <c r="M54" s="155"/>
+      <c r="N54" s="155"/>
       <c r="O54" s="18"/>
       <c r="P54" s="17"/>
     </row>
-    <row r="55" spans="1:16" s="59" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" s="59" customFormat="1" ht="13.9">
       <c r="A55" s="17"/>
       <c r="B55" s="18"/>
       <c r="C55" s="18"/>
@@ -4328,7 +4167,7 @@
       <c r="O55" s="18"/>
       <c r="P55" s="17"/>
     </row>
-    <row r="56" spans="1:16" s="59" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" s="59" customFormat="1" ht="13.9">
       <c r="A56" s="17"/>
       <c r="B56" s="17"/>
       <c r="C56" s="17"/>
@@ -4348,7 +4187,7 @@
     </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange algorithmName="SHA-512" hashValue="NcQe0VjxFnxU9SziGkmWOoYUYoQ0T62vv+WqFE1sowJD2+jDiq1RKEMS6wObDPCk433k/JG1CTU3j62rwNOzdg==" saltValue="OlYFZTFPx5QDCqKlqXj8fw==" spinCount="100000" sqref="C30:L30 C11:L12 D19:L19 N30 D29:E29 N15 C28 D14:L14 D15:E15 L15 C22:L23 D16:L17 G29:L29 D24:L27 C24:C26 D28:L28" name="Range1_2_1"/>
+    <protectedRange algorithmName="SHA-512" hashValue="NcQe0VjxFnxU9SziGkmWOoYUYoQ0T62vv+WqFE1sowJD2+jDiq1RKEMS6wObDPCk433k/JG1CTU3j62rwNOzdg==" saltValue="OlYFZTFPx5QDCqKlqXj8fw==" spinCount="100000" sqref="C30:L30 C11:L12 D19:L19 N30 D29:E29 N15 C28 D14:L14 D15:E15 L15 C22:L23 D16:L17 G29:L29 C24:C26 D24:L28" name="Range1_2_1"/>
     <protectedRange algorithmName="SHA-512" hashValue="NcQe0VjxFnxU9SziGkmWOoYUYoQ0T62vv+WqFE1sowJD2+jDiq1RKEMS6wObDPCk433k/JG1CTU3j62rwNOzdg==" saltValue="OlYFZTFPx5QDCqKlqXj8fw==" spinCount="100000" sqref="F29" name="Range1_2_1_2"/>
     <protectedRange algorithmName="SHA-512" hashValue="NcQe0VjxFnxU9SziGkmWOoYUYoQ0T62vv+WqFE1sowJD2+jDiq1RKEMS6wObDPCk433k/JG1CTU3j62rwNOzdg==" saltValue="OlYFZTFPx5QDCqKlqXj8fw==" spinCount="100000" sqref="D13:L13" name="Range1_2_1_1"/>
     <protectedRange algorithmName="SHA-512" hashValue="NcQe0VjxFnxU9SziGkmWOoYUYoQ0T62vv+WqFE1sowJD2+jDiq1RKEMS6wObDPCk433k/JG1CTU3j62rwNOzdg==" saltValue="OlYFZTFPx5QDCqKlqXj8fw==" spinCount="100000" sqref="D18:L18" name="Range1_2_1_3"/>
@@ -4439,183 +4278,100 @@
     <mergeCell ref="D44:E44"/>
     <mergeCell ref="G44:M44"/>
   </mergeCells>
-  <conditionalFormatting sqref="N4">
-    <cfRule type="containsText" dxfId="46" priority="94" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH(("FAIL"),(N4))))</formula>
+  <conditionalFormatting sqref="L29:L30">
+    <cfRule type="cellIs" dxfId="27" priority="42" operator="equal">
+      <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N4">
-    <cfRule type="cellIs" dxfId="45" priority="95" operator="equal">
-      <formula>"PASS"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N4">
-    <cfRule type="cellIs" dxfId="44" priority="96" operator="equal">
-      <formula>"M/O"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M17">
-    <cfRule type="cellIs" dxfId="43" priority="57" operator="equal">
+  <conditionalFormatting sqref="M14:M19">
+    <cfRule type="cellIs" dxfId="26" priority="20" operator="equal">
       <formula>"EXCELLENT"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="21" operator="equal">
       <formula>"GOOD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="22" operator="equal">
       <formula>"SUFFICIENT"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
       <formula>"INSUFFICIENT"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
       <formula>"MISSING"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M17">
-    <cfRule type="cellIs" dxfId="38" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
       <formula>"POOR"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L29">
-    <cfRule type="cellIs" dxfId="37" priority="73" operator="equal">
-      <formula>100</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M25 M19 M23">
-    <cfRule type="cellIs" dxfId="36" priority="69" operator="equal">
+  <conditionalFormatting sqref="M23 M25">
+    <cfRule type="cellIs" dxfId="20" priority="69" operator="equal">
       <formula>"EXCELLENT"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="70" operator="equal">
       <formula>"GOOD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="71" operator="equal">
       <formula>"SUFFICIENT"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="72" operator="equal">
       <formula>"INSUFFICIENT"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="74" operator="equal">
       <formula>"MISSING"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M25 M19 M23">
-    <cfRule type="cellIs" dxfId="31" priority="75" operator="equal">
-      <formula>"POOR"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L30">
-    <cfRule type="cellIs" dxfId="30" priority="42" operator="equal">
-      <formula>100</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M29">
-    <cfRule type="cellIs" dxfId="29" priority="38" operator="equal">
-      <formula>"EXCELLENT"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="39" operator="equal">
-      <formula>"GOOD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="40" operator="equal">
-      <formula>"SUFFICIENT"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="41" operator="equal">
-      <formula>"INSUFFICIENT"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="43" operator="equal">
-      <formula>"MISSING"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M29">
-    <cfRule type="cellIs" dxfId="24" priority="44" operator="equal">
-      <formula>"POOR"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M14:M15">
-    <cfRule type="cellIs" dxfId="23" priority="32" operator="equal">
-      <formula>"EXCELLENT"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="33" operator="equal">
-      <formula>"GOOD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="34" operator="equal">
-      <formula>"SUFFICIENT"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="35" operator="equal">
-      <formula>"INSUFFICIENT"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="36" operator="equal">
-      <formula>"MISSING"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M14:M15">
-    <cfRule type="cellIs" dxfId="18" priority="37" operator="equal">
-      <formula>"POOR"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M16">
-    <cfRule type="cellIs" dxfId="17" priority="26" operator="equal">
-      <formula>"EXCELLENT"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="27" operator="equal">
-      <formula>"GOOD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="28" operator="equal">
-      <formula>"SUFFICIENT"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="29" operator="equal">
-      <formula>"INSUFFICIENT"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="30" operator="equal">
-      <formula>"MISSING"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M16">
-    <cfRule type="cellIs" dxfId="12" priority="31" operator="equal">
-      <formula>"POOR"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M18">
-    <cfRule type="cellIs" dxfId="11" priority="20" operator="equal">
-      <formula>"EXCELLENT"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="21" operator="equal">
-      <formula>"GOOD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="22" operator="equal">
-      <formula>"SUFFICIENT"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="23" operator="equal">
-      <formula>"INSUFFICIENT"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="24" operator="equal">
-      <formula>"MISSING"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M18">
-    <cfRule type="cellIs" dxfId="6" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="75" operator="equal">
       <formula>"POOR"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M27">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
       <formula>"EXCELLENT"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
       <formula>"GOOD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
       <formula>"SUFFICIENT"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
       <formula>"INSUFFICIENT"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
       <formula>"MISSING"</formula>
     </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
+      <formula>"POOR"</formula>
+    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M27">
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+  <conditionalFormatting sqref="M29">
+    <cfRule type="cellIs" dxfId="8" priority="38" operator="equal">
+      <formula>"EXCELLENT"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="39" operator="equal">
+      <formula>"GOOD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="40" operator="equal">
+      <formula>"SUFFICIENT"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="41" operator="equal">
+      <formula>"INSUFFICIENT"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="43" operator="equal">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="44" operator="equal">
       <formula>"POOR"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N4">
+    <cfRule type="containsText" dxfId="2" priority="94" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH(("FAIL"),(N4))))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="95" operator="equal">
+      <formula>"PASS"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="96" operator="equal">
+      <formula>"M/O"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="1">
@@ -4633,11 +4389,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F364E9-2EB7-5940-933A-B5F5600966F3}">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="13.15"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="78"/>
     <col min="2" max="2" width="23.85546875" style="78" customWidth="1"/>
@@ -4650,50 +4406,50 @@
     <col min="9" max="16384" width="8.85546875" style="78"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="201" t="s">
-        <v>153</v>
-      </c>
-      <c r="B1" s="202"/>
-      <c r="C1" s="202"/>
-      <c r="D1" s="202"/>
-      <c r="E1" s="202"/>
-      <c r="F1" s="202"/>
-      <c r="G1" s="202"/>
-      <c r="H1" s="203"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="204"/>
-      <c r="B2" s="205"/>
-      <c r="C2" s="205"/>
-      <c r="D2" s="205"/>
-      <c r="E2" s="205"/>
-      <c r="F2" s="205"/>
-      <c r="G2" s="205"/>
-      <c r="H2" s="206"/>
-    </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="199" t="s">
-        <v>102</v>
-      </c>
-      <c r="B3" s="200"/>
+    <row r="1" spans="1:15">
+      <c r="A1" s="193" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" s="194"/>
+      <c r="C1" s="194"/>
+      <c r="D1" s="194"/>
+      <c r="E1" s="194"/>
+      <c r="F1" s="194"/>
+      <c r="G1" s="194"/>
+      <c r="H1" s="195"/>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="196"/>
+      <c r="B2" s="197"/>
+      <c r="C2" s="197"/>
+      <c r="D2" s="197"/>
+      <c r="E2" s="197"/>
+      <c r="F2" s="197"/>
+      <c r="G2" s="197"/>
+      <c r="H2" s="198"/>
+    </row>
+    <row r="3" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A3" s="191" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="192"/>
       <c r="C3" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="196" t="s">
-        <v>134</v>
-      </c>
-      <c r="E3" s="197"/>
-      <c r="F3" s="197"/>
-      <c r="G3" s="197"/>
-      <c r="H3" s="198"/>
-      <c r="K3" s="194"/>
-      <c r="L3" s="195"/>
-      <c r="M3" s="195"/>
-      <c r="N3" s="195"/>
+      <c r="D3" s="188" t="s">
+        <v>135</v>
+      </c>
+      <c r="E3" s="189"/>
+      <c r="F3" s="189"/>
+      <c r="G3" s="189"/>
+      <c r="H3" s="190"/>
+      <c r="K3" s="187"/>
+      <c r="L3" s="210"/>
+      <c r="M3" s="210"/>
+      <c r="N3" s="210"/>
       <c r="O3" s="100"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15">
       <c r="A4" s="99"/>
       <c r="B4" s="98"/>
       <c r="C4" s="98"/>
@@ -4713,25 +4469,25 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="26.45">
       <c r="A5" s="91"/>
       <c r="D5" s="94" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E5" s="93" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F5" s="93" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G5" s="93" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H5" s="92" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="91"/>
       <c r="D6" s="90"/>
       <c r="E6" s="89"/>
@@ -4739,278 +4495,278 @@
       <c r="G6" s="89"/>
       <c r="H6" s="88"/>
     </row>
-    <row r="7" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1">
       <c r="A7" s="105">
         <v>1</v>
       </c>
       <c r="B7" s="125" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C7" s="106" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D7" s="107" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E7" s="108" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F7" s="108" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G7" s="107" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H7" s="107" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1">
       <c r="A8" s="105">
         <v>2</v>
       </c>
       <c r="B8" s="125" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C8" s="132" t="s">
+        <v>159</v>
+      </c>
+      <c r="D8" s="107" t="s">
         <v>158</v>
       </c>
-      <c r="D8" s="107" t="s">
-        <v>157</v>
-      </c>
       <c r="E8" s="108" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F8" s="108" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G8" s="107"/>
       <c r="H8" s="107" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1">
       <c r="A9" s="133">
         <v>3</v>
       </c>
       <c r="B9" s="134" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C9" s="134" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D9" s="133" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E9" s="133" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F9" s="133" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G9" s="133" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H9" s="133" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1">
       <c r="A10" s="142">
         <v>4</v>
       </c>
       <c r="B10" s="143" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C10" s="143" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D10" s="144" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E10" s="145" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F10" s="145" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G10" s="144"/>
       <c r="H10" s="144" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1">
       <c r="A11" s="102">
         <v>5</v>
       </c>
       <c r="B11" s="104" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C11" s="104" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D11" s="102" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E11" s="102" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F11" s="102" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G11" s="102"/>
       <c r="H11" s="102" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1">
       <c r="A12" s="102">
         <v>6</v>
       </c>
       <c r="B12" s="103" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C12" s="104" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D12" s="102" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E12" s="102" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F12" s="102" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G12" s="102" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H12" s="102" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1">
       <c r="A13" s="102">
         <v>7</v>
       </c>
       <c r="B13" s="103" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C13" s="104" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D13" s="101" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E13" s="102" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F13" s="102" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G13" s="101" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H13" s="101"/>
     </row>
-    <row r="14" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1">
       <c r="A14" s="102">
         <v>8</v>
       </c>
       <c r="B14" s="103" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C14" s="104" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D14" s="101" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E14" s="102" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F14" s="102" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G14" s="101" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H14" s="101"/>
     </row>
-    <row r="15" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1">
       <c r="A15" s="87">
         <v>9</v>
       </c>
       <c r="B15" s="82" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C15" s="81" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D15" s="85" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E15" s="86" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F15" s="86" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G15" s="85" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H15" s="85"/>
     </row>
-    <row r="16" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1">
       <c r="A16" s="87">
         <v>10</v>
       </c>
       <c r="B16" s="82" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C16" s="81" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D16" s="85" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E16" s="86" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F16" s="86" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G16" s="85" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H16" s="85" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="80.099999999999994" customHeight="1">
       <c r="A17" s="83">
         <v>11</v>
       </c>
       <c r="B17" s="82" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C17" s="81" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D17" s="79" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E17" s="80" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F17" s="80" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G17" s="79" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H17" s="79" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -5033,42 +4789,42 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="7" max="7" width="18.140625" customWidth="1"/>
     <col min="9" max="9" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="26.45">
       <c r="A2" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="B2" s="209" t="s">
         <v>169</v>
       </c>
-      <c r="C2" s="177"/>
-      <c r="D2" s="177"/>
+      <c r="B2" s="201" t="s">
+        <v>170</v>
+      </c>
+      <c r="C2" s="205"/>
+      <c r="D2" s="205"/>
       <c r="G2" s="4"/>
       <c r="H2" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="13.9">
       <c r="B3" s="119"/>
       <c r="C3" s="119"/>
       <c r="D3" s="119"/>
@@ -5088,7 +4844,7 @@
       <c r="S3" s="2"/>
       <c r="T3" s="4"/>
     </row>
-    <row r="4" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="13.9">
       <c r="B4" s="119"/>
       <c r="C4" s="119"/>
       <c r="D4" s="119"/>
@@ -5108,35 +4864,35 @@
       <c r="S4" s="2"/>
       <c r="T4" s="4"/>
     </row>
-    <row r="5" spans="1:20" ht="191.25" x14ac:dyDescent="0.2">
-      <c r="B5" s="207" t="s">
-        <v>176</v>
-      </c>
-      <c r="C5" s="177"/>
-      <c r="D5" s="177"/>
+    <row r="5" spans="1:20" ht="184.9">
+      <c r="B5" s="199" t="s">
+        <v>177</v>
+      </c>
+      <c r="C5" s="205"/>
+      <c r="D5" s="205"/>
       <c r="F5" s="10">
         <v>6.1</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="N5" s="2" t="e">
         <f ca="1">_xludf.CONCAT(M5,M6)</f>
@@ -5164,28 +4920,28 @@
       </c>
       <c r="T5" s="4"/>
     </row>
-    <row r="6" spans="1:20" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" ht="105.6">
       <c r="B6" s="119"/>
       <c r="C6" s="119"/>
       <c r="D6" s="119"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -5195,35 +4951,35 @@
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
     </row>
-    <row r="7" spans="1:20" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="B7" s="207" t="s">
-        <v>190</v>
-      </c>
-      <c r="C7" s="177"/>
-      <c r="D7" s="177"/>
+    <row r="7" spans="1:20" ht="79.900000000000006">
+      <c r="B7" s="199" t="s">
+        <v>191</v>
+      </c>
+      <c r="C7" s="205"/>
+      <c r="D7" s="205"/>
       <c r="F7" s="10">
         <v>6.2</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="M7" s="8" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="N7" s="2" t="e">
         <f ca="1">_xludf.CONCAT(M7,M8)</f>
@@ -5251,30 +5007,30 @@
       </c>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="B8" s="207" t="s">
-        <v>198</v>
-      </c>
-      <c r="C8" s="177"/>
-      <c r="D8" s="177"/>
+    <row r="8" spans="1:20" ht="66.599999999999994">
+      <c r="B8" s="199" t="s">
+        <v>199</v>
+      </c>
+      <c r="C8" s="205"/>
+      <c r="D8" s="205"/>
       <c r="G8" s="4"/>
       <c r="H8" s="9" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
@@ -5284,7 +5040,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" ht="13.15">
       <c r="G9" s="10"/>
       <c r="H9" s="4"/>
       <c r="I9" s="10"/>
@@ -5292,7 +5048,7 @@
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
     </row>
-    <row r="10" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" ht="13.15">
       <c r="G10" s="10"/>
       <c r="H10" s="4"/>
       <c r="I10" s="10"/>
@@ -5301,7 +5057,7 @@
       <c r="L10" s="10"/>
       <c r="M10" s="11"/>
     </row>
-    <row r="11" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" ht="13.15">
       <c r="G11" s="10"/>
       <c r="H11" s="4"/>
       <c r="I11" s="10"/>
@@ -5310,7 +5066,7 @@
       <c r="L11" s="10"/>
       <c r="M11" s="11"/>
     </row>
-    <row r="12" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" ht="13.15">
       <c r="G12" s="10"/>
       <c r="H12" s="4"/>
       <c r="I12" s="10"/>
@@ -5319,57 +5075,57 @@
       <c r="L12" s="10"/>
       <c r="M12" s="11"/>
     </row>
-    <row r="13" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B13" s="208"/>
-      <c r="C13" s="177"/>
-      <c r="D13" s="177"/>
+    <row r="13" spans="1:20" ht="13.9">
+      <c r="B13" s="200"/>
+      <c r="C13" s="205"/>
+      <c r="D13" s="205"/>
       <c r="G13" s="10"/>
       <c r="H13" s="4" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="L13" s="10" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="M13" s="11" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="207" t="s">
         <v>210</v>
       </c>
-      <c r="C14" s="177"/>
-      <c r="D14" s="177"/>
+    </row>
+    <row r="14" spans="1:20" ht="70.5" customHeight="1">
+      <c r="B14" s="199" t="s">
+        <v>211</v>
+      </c>
+      <c r="C14" s="205"/>
+      <c r="D14" s="205"/>
       <c r="F14" s="10">
         <v>3.1</v>
       </c>
       <c r="G14" s="12"/>
       <c r="H14" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="N14" s="2" t="e">
         <f ca="1">_xludf.CONCAT(M14,M15)</f>
@@ -5396,31 +5152,31 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" ht="66.75" customHeight="1">
       <c r="B15" s="13"/>
       <c r="G15" s="12" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="13.15">
       <c r="G16" s="10"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
@@ -5429,7 +5185,7 @@
       <c r="L16" s="4"/>
       <c r="M16" s="14"/>
     </row>
-    <row r="17" spans="2:19" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:19" ht="13.15">
       <c r="G17" s="10"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
@@ -5438,33 +5194,33 @@
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
     </row>
-    <row r="18" spans="2:19" ht="255" x14ac:dyDescent="0.2">
-      <c r="B18" s="207" t="s">
-        <v>222</v>
-      </c>
-      <c r="C18" s="177"/>
-      <c r="D18" s="177"/>
+    <row r="18" spans="2:19" ht="251.45">
+      <c r="B18" s="199" t="s">
+        <v>223</v>
+      </c>
+      <c r="C18" s="205"/>
+      <c r="D18" s="205"/>
       <c r="F18" s="10">
         <v>3.2</v>
       </c>
       <c r="G18" s="10"/>
       <c r="H18" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="N18" s="4" t="e">
         <f ca="1">_xludf.CONCAT(M18,M19)</f>
@@ -5491,22 +5247,22 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="19" spans="2:19" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:19" ht="132">
       <c r="G19" s="10"/>
       <c r="H19" s="9" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="M19" s="4"/>
     </row>
-    <row r="20" spans="2:19" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:19" ht="13.15">
       <c r="G20" s="10"/>
       <c r="H20" s="4"/>
       <c r="I20" s="10"/>
@@ -5515,7 +5271,7 @@
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
     </row>
-    <row r="21" spans="2:19" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:19" ht="13.15">
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
@@ -5524,7 +5280,7 @@
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
     </row>
-    <row r="22" spans="2:19" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:19" ht="13.15">
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
@@ -5533,57 +5289,57 @@
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
     </row>
-    <row r="24" spans="2:19" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:19" ht="13.15">
       <c r="H24" s="10" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="K24" s="10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="L24" s="10" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="M24" s="10" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="25" spans="2:19" ht="280.5" x14ac:dyDescent="0.2">
-      <c r="B25" s="208" t="s">
         <v>234</v>
       </c>
-      <c r="C25" s="177"/>
-      <c r="D25" s="177"/>
+    </row>
+    <row r="25" spans="2:19" ht="290.45">
+      <c r="B25" s="200" t="s">
+        <v>235</v>
+      </c>
+      <c r="C25" s="205"/>
+      <c r="D25" s="205"/>
       <c r="G25" s="10" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="26" spans="2:19" ht="12.75" x14ac:dyDescent="0.2">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="26" spans="2:19" ht="13.15">
       <c r="G26" s="10" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -5603,25 +5359,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bd38d267-56bb-4e22-b975-199a06fd69fa">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d8c712e5-67fc-4595-93cb-a4164dd8eff3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DB06FA0A2AD4DA488583749EC2534234" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="886b513cfe8a01d235b598bb5d9e3280">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="60348849-ecd6-40c5-8069-7b4f665118aa" xmlns:ns3="d3efc331-58f4-463c-b792-81d907c25a2d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ea6c152a0770c3b66e26597cca1a51d2" ns2:_="" ns3:_="">
-    <xsd:import namespace="60348849-ecd6-40c5-8069-7b4f665118aa"/>
-    <xsd:import namespace="d3efc331-58f4-463c-b792-81d907c25a2d"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010064DEF28CA2629948A9F801C782641252" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4e29c08bd2fa8ab5d37e806398c14b17">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bd38d267-56bb-4e22-b975-199a06fd69fa" xmlns:ns3="d8c712e5-67fc-4595-93cb-a4164dd8eff3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="30fadebd201830d804edab1b035af467" ns2:_="" ns3:_="">
+    <xsd:import namespace="bd38d267-56bb-4e22-b975-199a06fd69fa"/>
+    <xsd:import namespace="d8c712e5-67fc-4595-93cb-a4164dd8eff3"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -5630,16 +5382,21 @@
               <xsd:all>
                 <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -5647,7 +5404,7 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="60348849-ecd6-40c5-8069-7b4f665118aa" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="bd38d267-56bb-4e22-b975-199a06fd69fa" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
@@ -5660,16 +5417,14 @@
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
       <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+    <xsd:element name="MediaLengthInSeconds" ma:index="11" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
       <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
+        <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
     <xsd:element name="MediaServiceAutoTags" ma:index="12" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
@@ -5677,11 +5432,9 @@
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+    <xsd:element name="MediaServiceLocation" ma:index="13" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
       <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
     <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
@@ -5694,18 +5447,44 @@
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="16" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="17" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="21" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="365a90ea-d0e7-4aae-8ef9-9f5dd1eb65e3" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="23" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="24" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="25" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="17" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="d3efc331-58f4-463c-b792-81d907c25a2d" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="d8c712e5-67fc-4595-93cb-a4164dd8eff3" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="SharedWithUsers" ma:index="18" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
@@ -5733,6 +5512,17 @@
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="22" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{5e624992-a676-4554-99c9-a3d8ae70b3e3}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="d8c712e5-67fc-4595-93cb-a4164dd8eff3">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -5834,38 +5624,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BB72468-B9EB-412A-8D55-6151E9A308C0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D98D897-3D5D-4CF5-A274-8B2E15AE73B2}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D98D897-3D5D-4CF5-A274-8B2E15AE73B2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{873E3095-4F4D-4DD9-BAD5-E276899012AF}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCA8CA2F-1DC9-4462-8B83-EF7474A9E105}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="60348849-ecd6-40c5-8069-7b4f665118aa"/>
-    <ds:schemaRef ds:uri="d3efc331-58f4-463c-b792-81d907c25a2d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BB72468-B9EB-412A-8D55-6151E9A308C0}"/>
 </file>
</xml_diff>

<commit_message>
Update Self-Assessment Rubric Block - Y1D_2022-23_ADSAI.xlsx
</commit_message>
<xml_diff>
--- a/docs/Year1/BlockD/MS Assignment Template/Self-Assessment Rubric Block - Y1D_2022-23_ADSAI.xlsx
+++ b/docs/Year1/BlockD/MS Assignment Template/Self-Assessment Rubric Block - Y1D_2022-23_ADSAI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://edubuas.sharepoint.com/teams/ADSAI2022-23/Shared Documents/General/Design documentation/Year 1 Design/Block D/MS Teams Assignment Template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bramh\Documents\GitHub\AAI-DM\docs\Year1\BlockD\MS Assignment Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="678" documentId="11_03746045E4F30D67E4D3283C82E484B242FC1AB4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35BEF582-8A36-474F-B837-16F776521440}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D35BE435-797F-4962-9218-D94C26979C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1068" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51480" yWindow="3495" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Student Self-Assessment" sheetId="6" r:id="rId1"/>
@@ -846,7 +846,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="29">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2002,78 +2002,46 @@
     <xf numFmtId="0" fontId="19" fillId="56" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="53" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="27" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="53" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="53" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -2112,24 +2080,65 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="53" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -2172,19 +2181,10 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{9902F182-0AFB-1F41-B571-EB1D4AC04E32}"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="34">
     <dxf>
@@ -2678,11 +2678,11 @@
   <dimension ref="A1:P56"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D29" sqref="D29:E29"/>
+      <pane ySplit="10" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.42578125" style="39" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" style="39" customWidth="1"/>
@@ -2700,7 +2700,7 @@
     <col min="17" max="16384" width="14.42578125" style="39"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="12.95" customHeight="1">
+    <row r="1" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="17"/>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -2718,14 +2718,14 @@
       <c r="O1" s="17"/>
       <c r="P1" s="17"/>
     </row>
-    <row r="2" spans="1:16" ht="23.45">
+    <row r="2" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="17"/>
       <c r="B2" s="18"/>
-      <c r="C2" s="202" t="s">
+      <c r="C2" s="152" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="203"/>
-      <c r="E2" s="203"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="153"/>
       <c r="F2" s="18"/>
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
@@ -2738,11 +2738,11 @@
       <c r="O2" s="18"/>
       <c r="P2" s="17"/>
     </row>
-    <row r="3" spans="1:16" s="23" customFormat="1" ht="14.45" customHeight="1">
+    <row r="3" spans="1:16" s="23" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="19"/>
       <c r="B3" s="20"/>
-      <c r="C3" s="169"/>
-      <c r="D3" s="204"/>
+      <c r="C3" s="158"/>
+      <c r="D3" s="159"/>
       <c r="E3" s="38" t="s">
         <v>1</v>
       </c>
@@ -2752,135 +2752,135 @@
       <c r="G3" s="21"/>
       <c r="H3" s="22"/>
       <c r="I3" s="22"/>
-      <c r="J3" s="153" t="s">
+      <c r="J3" s="160" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="205"/>
-      <c r="L3" s="170" t="s">
+      <c r="K3" s="161"/>
+      <c r="L3" s="162" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="203"/>
-      <c r="N3" s="203"/>
+      <c r="M3" s="153"/>
+      <c r="N3" s="153"/>
       <c r="O3" s="20"/>
       <c r="P3" s="19"/>
     </row>
-    <row r="4" spans="1:16" ht="12.95" customHeight="1">
+    <row r="4" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17"/>
       <c r="B4" s="24"/>
-      <c r="C4" s="171" t="s">
+      <c r="C4" s="163" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="203"/>
+      <c r="D4" s="153"/>
       <c r="E4" s="15"/>
-      <c r="F4" s="172" t="s">
+      <c r="F4" s="164" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="173"/>
-      <c r="H4" s="173"/>
-      <c r="I4" s="173"/>
-      <c r="J4" s="174"/>
-      <c r="K4" s="175"/>
-      <c r="L4" s="176" t="s">
+      <c r="G4" s="165"/>
+      <c r="H4" s="165"/>
+      <c r="I4" s="165"/>
+      <c r="J4" s="166"/>
+      <c r="K4" s="167"/>
+      <c r="L4" s="168" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="177">
+      <c r="M4" s="169">
         <f>IF(ROUND((N29/10),1)&lt;&gt;ROUND((N29/10),0),ROUND((N29/10),1),ROUND((N29/10),0))</f>
         <v>0</v>
       </c>
-      <c r="N4" s="178" t="str">
+      <c r="N4" s="170" t="str">
         <f>IF(M4&gt;=5.5,"PASS",IF(M4&gt;0,"FAIL","M/O"))</f>
         <v>M/O</v>
       </c>
       <c r="O4" s="18"/>
       <c r="P4" s="17"/>
     </row>
-    <row r="5" spans="1:16" ht="12.95" customHeight="1">
+    <row r="5" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="17"/>
       <c r="B5" s="24"/>
-      <c r="C5" s="171" t="s">
+      <c r="C5" s="163" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="205"/>
+      <c r="D5" s="161"/>
       <c r="E5" s="15"/>
-      <c r="F5" s="173"/>
-      <c r="G5" s="173"/>
-      <c r="H5" s="173"/>
-      <c r="I5" s="173"/>
-      <c r="J5" s="175"/>
-      <c r="K5" s="175"/>
-      <c r="L5" s="205"/>
-      <c r="M5" s="205"/>
-      <c r="N5" s="205"/>
+      <c r="F5" s="165"/>
+      <c r="G5" s="165"/>
+      <c r="H5" s="165"/>
+      <c r="I5" s="165"/>
+      <c r="J5" s="167"/>
+      <c r="K5" s="167"/>
+      <c r="L5" s="161"/>
+      <c r="M5" s="161"/>
+      <c r="N5" s="161"/>
       <c r="O5" s="18"/>
       <c r="P5" s="17"/>
     </row>
-    <row r="6" spans="1:16" ht="13.9">
+    <row r="6" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="17"/>
       <c r="B6" s="24"/>
-      <c r="C6" s="171" t="s">
+      <c r="C6" s="163" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="179"/>
+      <c r="D6" s="171"/>
       <c r="E6" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="173"/>
-      <c r="G6" s="173"/>
-      <c r="H6" s="173"/>
-      <c r="I6" s="173"/>
-      <c r="J6" s="175"/>
-      <c r="K6" s="175"/>
-      <c r="L6" s="205"/>
-      <c r="M6" s="205"/>
-      <c r="N6" s="205"/>
+      <c r="F6" s="165"/>
+      <c r="G6" s="165"/>
+      <c r="H6" s="165"/>
+      <c r="I6" s="165"/>
+      <c r="J6" s="167"/>
+      <c r="K6" s="167"/>
+      <c r="L6" s="161"/>
+      <c r="M6" s="161"/>
+      <c r="N6" s="161"/>
       <c r="O6" s="18"/>
       <c r="P6" s="17"/>
     </row>
-    <row r="7" spans="1:16" ht="13.9">
+    <row r="7" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="17"/>
       <c r="B7" s="24"/>
-      <c r="C7" s="171" t="s">
+      <c r="C7" s="163" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="205"/>
+      <c r="D7" s="161"/>
       <c r="E7" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="173"/>
-      <c r="G7" s="173"/>
-      <c r="H7" s="173"/>
-      <c r="I7" s="173"/>
-      <c r="J7" s="175"/>
-      <c r="K7" s="175"/>
-      <c r="L7" s="205"/>
-      <c r="M7" s="205"/>
-      <c r="N7" s="205"/>
+      <c r="F7" s="165"/>
+      <c r="G7" s="165"/>
+      <c r="H7" s="165"/>
+      <c r="I7" s="165"/>
+      <c r="J7" s="167"/>
+      <c r="K7" s="167"/>
+      <c r="L7" s="161"/>
+      <c r="M7" s="161"/>
+      <c r="N7" s="161"/>
       <c r="O7" s="18"/>
       <c r="P7" s="17"/>
     </row>
-    <row r="8" spans="1:16" ht="28.35" customHeight="1">
+    <row r="8" spans="1:16" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17"/>
       <c r="B8" s="24"/>
-      <c r="C8" s="180" t="s">
+      <c r="C8" s="172" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="181"/>
+      <c r="D8" s="173"/>
       <c r="E8" s="131" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="173"/>
-      <c r="G8" s="173"/>
-      <c r="H8" s="173"/>
-      <c r="I8" s="173"/>
-      <c r="J8" s="175"/>
-      <c r="K8" s="175"/>
-      <c r="L8" s="205"/>
-      <c r="M8" s="205"/>
-      <c r="N8" s="205"/>
+      <c r="F8" s="165"/>
+      <c r="G8" s="165"/>
+      <c r="H8" s="165"/>
+      <c r="I8" s="165"/>
+      <c r="J8" s="167"/>
+      <c r="K8" s="167"/>
+      <c r="L8" s="161"/>
+      <c r="M8" s="161"/>
+      <c r="N8" s="161"/>
       <c r="O8" s="18"/>
       <c r="P8" s="17"/>
     </row>
-    <row r="9" spans="1:16" ht="13.9">
+    <row r="9" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="17"/>
       <c r="B9" s="18"/>
       <c r="C9" s="18"/>
@@ -2898,7 +2898,7 @@
       <c r="O9" s="18"/>
       <c r="P9" s="17"/>
     </row>
-    <row r="10" spans="1:16" ht="13.9">
+    <row r="10" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
@@ -2916,14 +2916,14 @@
       <c r="O10" s="17"/>
       <c r="P10" s="17"/>
     </row>
-    <row r="11" spans="1:16" ht="23.45">
+    <row r="11" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A11" s="17"/>
       <c r="B11" s="18"/>
-      <c r="C11" s="202" t="s">
+      <c r="C11" s="152" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="203"/>
-      <c r="E11" s="203"/>
+      <c r="D11" s="153"/>
+      <c r="E11" s="153"/>
       <c r="F11" s="18"/>
       <c r="G11" s="18"/>
       <c r="H11" s="18"/>
@@ -2936,7 +2936,7 @@
       <c r="O11" s="18"/>
       <c r="P11" s="17"/>
     </row>
-    <row r="12" spans="1:16" ht="13.9">
+    <row r="12" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="17"/>
       <c r="B12" s="18"/>
       <c r="C12" s="42"/>
@@ -2974,36 +2974,36 @@
       <c r="O12" s="26"/>
       <c r="P12" s="17"/>
     </row>
-    <row r="13" spans="1:16" ht="48.95" customHeight="1">
+    <row r="13" spans="1:16" ht="48.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="17"/>
       <c r="B13" s="27"/>
-      <c r="C13" s="161" t="s">
+      <c r="C13" s="151" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="184" t="s">
+      <c r="D13" s="154" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="163"/>
-      <c r="F13" s="163"/>
-      <c r="G13" s="163"/>
-      <c r="H13" s="163"/>
-      <c r="I13" s="163"/>
-      <c r="J13" s="163"/>
-      <c r="K13" s="163"/>
+      <c r="E13" s="148"/>
+      <c r="F13" s="148"/>
+      <c r="G13" s="148"/>
+      <c r="H13" s="148"/>
+      <c r="I13" s="148"/>
+      <c r="J13" s="148"/>
+      <c r="K13" s="148"/>
       <c r="L13" s="120"/>
       <c r="M13" s="120"/>
       <c r="N13" s="120"/>
       <c r="O13" s="28"/>
       <c r="P13" s="17"/>
     </row>
-    <row r="14" spans="1:16" ht="118.9" customHeight="1">
+    <row r="14" spans="1:16" ht="118.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="17"/>
       <c r="B14" s="27"/>
-      <c r="C14" s="161"/>
-      <c r="D14" s="164" t="s">
+      <c r="C14" s="151"/>
+      <c r="D14" s="156" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="164"/>
+      <c r="E14" s="156"/>
       <c r="F14" s="57" t="s">
         <v>29</v>
       </c>
@@ -3035,14 +3035,14 @@
       <c r="O14" s="28"/>
       <c r="P14" s="17"/>
     </row>
-    <row r="15" spans="1:16" ht="105.95" customHeight="1">
+    <row r="15" spans="1:16" ht="105.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="17"/>
       <c r="B15" s="27"/>
-      <c r="C15" s="161"/>
-      <c r="D15" s="164" t="s">
+      <c r="C15" s="151"/>
+      <c r="D15" s="156" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="164"/>
+      <c r="E15" s="156"/>
       <c r="F15" s="57" t="s">
         <v>29</v>
       </c>
@@ -3073,14 +3073,14 @@
       <c r="O15" s="28"/>
       <c r="P15" s="17"/>
     </row>
-    <row r="16" spans="1:16" ht="116.45" customHeight="1">
+    <row r="16" spans="1:16" ht="116.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="17"/>
       <c r="B16" s="27"/>
-      <c r="C16" s="161"/>
-      <c r="D16" s="164" t="s">
+      <c r="C16" s="151"/>
+      <c r="D16" s="156" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="164"/>
+      <c r="E16" s="156"/>
       <c r="F16" s="57" t="s">
         <v>29</v>
       </c>
@@ -3112,14 +3112,14 @@
       <c r="O16" s="28"/>
       <c r="P16" s="17"/>
     </row>
-    <row r="17" spans="1:16" ht="118.15" customHeight="1">
+    <row r="17" spans="1:16" ht="118.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="17"/>
       <c r="B17" s="18"/>
-      <c r="C17" s="161"/>
-      <c r="D17" s="164" t="s">
+      <c r="C17" s="151"/>
+      <c r="D17" s="156" t="s">
         <v>47</v>
       </c>
-      <c r="E17" s="164"/>
+      <c r="E17" s="156"/>
       <c r="F17" s="57" t="s">
         <v>29</v>
       </c>
@@ -3151,36 +3151,36 @@
       <c r="O17" s="28"/>
       <c r="P17" s="17"/>
     </row>
-    <row r="18" spans="1:16" ht="48.6" customHeight="1">
+    <row r="18" spans="1:16" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="17"/>
       <c r="B18" s="27"/>
-      <c r="C18" s="160" t="s">
+      <c r="C18" s="146" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="184" t="s">
+      <c r="D18" s="154" t="s">
         <v>54</v>
       </c>
-      <c r="E18" s="185"/>
-      <c r="F18" s="185"/>
-      <c r="G18" s="185"/>
-      <c r="H18" s="185"/>
-      <c r="I18" s="185"/>
-      <c r="J18" s="185"/>
-      <c r="K18" s="185"/>
+      <c r="E18" s="155"/>
+      <c r="F18" s="155"/>
+      <c r="G18" s="155"/>
+      <c r="H18" s="155"/>
+      <c r="I18" s="155"/>
+      <c r="J18" s="155"/>
+      <c r="K18" s="155"/>
       <c r="L18" s="121"/>
       <c r="M18" s="121"/>
       <c r="N18" s="121"/>
       <c r="O18" s="28"/>
       <c r="P18" s="17"/>
     </row>
-    <row r="19" spans="1:16" ht="118.7" customHeight="1">
+    <row r="19" spans="1:16" ht="118.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="17"/>
       <c r="B19" s="18"/>
-      <c r="C19" s="160"/>
-      <c r="D19" s="186" t="s">
+      <c r="C19" s="146"/>
+      <c r="D19" s="157" t="s">
         <v>55</v>
       </c>
-      <c r="E19" s="186"/>
+      <c r="E19" s="157"/>
       <c r="F19" s="123" t="s">
         <v>29</v>
       </c>
@@ -3212,36 +3212,36 @@
       <c r="O19" s="28"/>
       <c r="P19" s="17"/>
     </row>
-    <row r="20" spans="1:16" s="59" customFormat="1" ht="48" customHeight="1">
+    <row r="20" spans="1:16" s="59" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="17"/>
       <c r="B20" s="27"/>
-      <c r="C20" s="160" t="s">
+      <c r="C20" s="146" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="162" t="s">
+      <c r="D20" s="147" t="s">
         <v>62</v>
       </c>
-      <c r="E20" s="163"/>
-      <c r="F20" s="163"/>
-      <c r="G20" s="163"/>
-      <c r="H20" s="163"/>
-      <c r="I20" s="163"/>
-      <c r="J20" s="163"/>
-      <c r="K20" s="163"/>
+      <c r="E20" s="148"/>
+      <c r="F20" s="148"/>
+      <c r="G20" s="148"/>
+      <c r="H20" s="148"/>
+      <c r="I20" s="148"/>
+      <c r="J20" s="148"/>
+      <c r="K20" s="148"/>
       <c r="L20" s="122"/>
       <c r="M20" s="122"/>
       <c r="N20" s="122"/>
       <c r="O20" s="28"/>
       <c r="P20" s="17"/>
     </row>
-    <row r="21" spans="1:16" s="59" customFormat="1" ht="136.5" customHeight="1">
+    <row r="21" spans="1:16" s="59" customFormat="1" ht="136.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="17"/>
       <c r="B21" s="18"/>
-      <c r="C21" s="160"/>
-      <c r="D21" s="182" t="s">
+      <c r="C21" s="146"/>
+      <c r="D21" s="149" t="s">
         <v>63</v>
       </c>
-      <c r="E21" s="183"/>
+      <c r="E21" s="150"/>
       <c r="F21" s="57" t="s">
         <v>64</v>
       </c>
@@ -3273,36 +3273,36 @@
       <c r="O21" s="28"/>
       <c r="P21" s="17"/>
     </row>
-    <row r="22" spans="1:16" ht="48" customHeight="1">
+    <row r="22" spans="1:16" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17"/>
       <c r="B22" s="27"/>
-      <c r="C22" s="160" t="s">
+      <c r="C22" s="146" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="162" t="s">
+      <c r="D22" s="147" t="s">
         <v>71</v>
       </c>
-      <c r="E22" s="163"/>
-      <c r="F22" s="163"/>
-      <c r="G22" s="163"/>
-      <c r="H22" s="163"/>
-      <c r="I22" s="163"/>
-      <c r="J22" s="163"/>
-      <c r="K22" s="163"/>
+      <c r="E22" s="148"/>
+      <c r="F22" s="148"/>
+      <c r="G22" s="148"/>
+      <c r="H22" s="148"/>
+      <c r="I22" s="148"/>
+      <c r="J22" s="148"/>
+      <c r="K22" s="148"/>
       <c r="L22" s="122"/>
       <c r="M22" s="122"/>
       <c r="N22" s="122"/>
       <c r="O22" s="28"/>
       <c r="P22" s="17"/>
     </row>
-    <row r="23" spans="1:16" ht="108" customHeight="1">
+    <row r="23" spans="1:16" ht="108" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="17"/>
       <c r="B23" s="18"/>
-      <c r="C23" s="160"/>
-      <c r="D23" s="164" t="s">
+      <c r="C23" s="146"/>
+      <c r="D23" s="156" t="s">
         <v>72</v>
       </c>
-      <c r="E23" s="165"/>
+      <c r="E23" s="174"/>
       <c r="F23" s="139" t="s">
         <v>64</v>
       </c>
@@ -3334,36 +3334,36 @@
       <c r="O23" s="28"/>
       <c r="P23" s="17"/>
     </row>
-    <row r="24" spans="1:16" ht="42.95" customHeight="1">
+    <row r="24" spans="1:16" ht="42.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="17"/>
       <c r="B24" s="27"/>
-      <c r="C24" s="161" t="s">
+      <c r="C24" s="151" t="s">
         <v>78</v>
       </c>
-      <c r="D24" s="166" t="s">
+      <c r="D24" s="175" t="s">
         <v>79</v>
       </c>
-      <c r="E24" s="166"/>
-      <c r="F24" s="166"/>
-      <c r="G24" s="166"/>
-      <c r="H24" s="166"/>
-      <c r="I24" s="166"/>
-      <c r="J24" s="166"/>
-      <c r="K24" s="166"/>
+      <c r="E24" s="175"/>
+      <c r="F24" s="175"/>
+      <c r="G24" s="175"/>
+      <c r="H24" s="175"/>
+      <c r="I24" s="175"/>
+      <c r="J24" s="175"/>
+      <c r="K24" s="175"/>
       <c r="L24" s="45"/>
       <c r="M24" s="45"/>
       <c r="N24" s="45"/>
       <c r="O24" s="28"/>
       <c r="P24" s="17"/>
     </row>
-    <row r="25" spans="1:16" s="56" customFormat="1" ht="144" customHeight="1">
+    <row r="25" spans="1:16" s="56" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="48"/>
       <c r="B25" s="49"/>
-      <c r="C25" s="203"/>
-      <c r="D25" s="167" t="s">
+      <c r="C25" s="153"/>
+      <c r="D25" s="176" t="s">
         <v>80</v>
       </c>
-      <c r="E25" s="167"/>
+      <c r="E25" s="176"/>
       <c r="F25" s="64" t="s">
         <v>29</v>
       </c>
@@ -3395,20 +3395,20 @@
       <c r="O25" s="55"/>
       <c r="P25" s="48"/>
     </row>
-    <row r="26" spans="1:16" ht="53.1" customHeight="1">
+    <row r="26" spans="1:16" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="17"/>
       <c r="B26" s="18"/>
-      <c r="C26" s="160" t="s">
+      <c r="C26" s="146" t="s">
         <v>86</v>
       </c>
-      <c r="D26" s="162" t="s">
+      <c r="D26" s="147" t="s">
         <v>87</v>
       </c>
-      <c r="E26" s="162"/>
-      <c r="F26" s="162"/>
-      <c r="G26" s="162"/>
-      <c r="H26" s="162"/>
-      <c r="I26" s="162"/>
+      <c r="E26" s="147"/>
+      <c r="F26" s="147"/>
+      <c r="G26" s="147"/>
+      <c r="H26" s="147"/>
+      <c r="I26" s="147"/>
       <c r="J26" s="113"/>
       <c r="K26" s="113"/>
       <c r="L26" s="122"/>
@@ -3417,14 +3417,14 @@
       <c r="O26" s="28"/>
       <c r="P26" s="17"/>
     </row>
-    <row r="27" spans="1:16" ht="111" customHeight="1">
+    <row r="27" spans="1:16" ht="111" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="17"/>
       <c r="B27" s="18"/>
-      <c r="C27" s="160"/>
-      <c r="D27" s="164" t="s">
+      <c r="C27" s="146"/>
+      <c r="D27" s="156" t="s">
         <v>88</v>
       </c>
-      <c r="E27" s="164"/>
+      <c r="E27" s="156"/>
       <c r="F27" s="57" t="s">
         <v>64</v>
       </c>
@@ -3456,36 +3456,36 @@
       <c r="O27" s="28"/>
       <c r="P27" s="17"/>
     </row>
-    <row r="28" spans="1:16" ht="53.1" customHeight="1">
+    <row r="28" spans="1:16" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="17"/>
       <c r="B28" s="18"/>
-      <c r="C28" s="160" t="s">
+      <c r="C28" s="146" t="s">
         <v>93</v>
       </c>
-      <c r="D28" s="168" t="s">
+      <c r="D28" s="177" t="s">
         <v>94</v>
       </c>
-      <c r="E28" s="168"/>
-      <c r="F28" s="168"/>
-      <c r="G28" s="168"/>
-      <c r="H28" s="168"/>
-      <c r="I28" s="168"/>
-      <c r="J28" s="168"/>
-      <c r="K28" s="168"/>
+      <c r="E28" s="177"/>
+      <c r="F28" s="177"/>
+      <c r="G28" s="177"/>
+      <c r="H28" s="177"/>
+      <c r="I28" s="177"/>
+      <c r="J28" s="177"/>
+      <c r="K28" s="177"/>
       <c r="L28" s="122"/>
       <c r="M28" s="122"/>
       <c r="N28" s="122"/>
       <c r="O28" s="28"/>
       <c r="P28" s="17"/>
     </row>
-    <row r="29" spans="1:16" s="63" customFormat="1" ht="150" customHeight="1">
+    <row r="29" spans="1:16" s="63" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="60"/>
       <c r="B29" s="61"/>
-      <c r="C29" s="160"/>
-      <c r="D29" s="164" t="s">
+      <c r="C29" s="146"/>
+      <c r="D29" s="156" t="s">
         <v>95</v>
       </c>
-      <c r="E29" s="164"/>
+      <c r="E29" s="156"/>
       <c r="F29" s="57" t="s">
         <v>64</v>
       </c>
@@ -3517,7 +3517,7 @@
       <c r="O29" s="62"/>
       <c r="P29" s="60"/>
     </row>
-    <row r="30" spans="1:16" ht="35.85" customHeight="1">
+    <row r="30" spans="1:16" ht="35.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
       <c r="B30" s="27"/>
       <c r="C30" s="18"/>
@@ -3545,7 +3545,7 @@
       <c r="O30" s="28"/>
       <c r="P30" s="17"/>
     </row>
-    <row r="31" spans="1:16" ht="17.45" customHeight="1">
+    <row r="31" spans="1:16" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
       <c r="B31" s="18"/>
       <c r="C31" s="18"/>
@@ -3563,7 +3563,7 @@
       <c r="O31" s="28"/>
       <c r="P31" s="17"/>
     </row>
-    <row r="32" spans="1:16" s="59" customFormat="1" ht="13.9">
+    <row r="32" spans="1:16" s="59" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="17"/>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
@@ -3581,14 +3581,14 @@
       <c r="O32" s="17"/>
       <c r="P32" s="17"/>
     </row>
-    <row r="33" spans="1:16" s="59" customFormat="1" ht="23.45">
+    <row r="33" spans="1:16" s="59" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A33" s="17"/>
       <c r="B33" s="29"/>
-      <c r="C33" s="202" t="s">
+      <c r="C33" s="152" t="s">
         <v>103</v>
       </c>
-      <c r="D33" s="203"/>
-      <c r="E33" s="203"/>
+      <c r="D33" s="153"/>
+      <c r="E33" s="153"/>
       <c r="F33" s="29"/>
       <c r="G33" s="29"/>
       <c r="H33" s="29"/>
@@ -3601,26 +3601,26 @@
       <c r="O33" s="30"/>
       <c r="P33" s="17"/>
     </row>
-    <row r="34" spans="1:16" s="59" customFormat="1" ht="13.9">
+    <row r="34" spans="1:16" s="59" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
       <c r="B34" s="29"/>
       <c r="C34" s="109" t="s">
         <v>104</v>
       </c>
-      <c r="D34" s="153" t="s">
+      <c r="D34" s="160" t="s">
         <v>105</v>
       </c>
-      <c r="E34" s="203"/>
+      <c r="E34" s="153"/>
       <c r="F34" s="109" t="s">
         <v>106</v>
       </c>
-      <c r="G34" s="153" t="s">
+      <c r="G34" s="160" t="s">
         <v>2</v>
       </c>
-      <c r="H34" s="203"/>
-      <c r="I34" s="203"/>
-      <c r="J34" s="203"/>
-      <c r="K34" s="203"/>
+      <c r="H34" s="153"/>
+      <c r="I34" s="153"/>
+      <c r="J34" s="153"/>
+      <c r="K34" s="153"/>
       <c r="L34" s="65"/>
       <c r="M34" s="109"/>
       <c r="N34" s="110" t="s">
@@ -3629,315 +3629,315 @@
       <c r="O34" s="29"/>
       <c r="P34" s="17"/>
     </row>
-    <row r="35" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1">
+    <row r="35" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="17"/>
       <c r="B35" s="29"/>
       <c r="C35" s="66">
         <v>9</v>
       </c>
-      <c r="D35" s="159" t="s">
+      <c r="D35" s="178" t="s">
         <v>108</v>
       </c>
-      <c r="E35" s="206"/>
+      <c r="E35" s="179"/>
       <c r="F35" s="111" t="s">
         <v>109</v>
       </c>
-      <c r="G35" s="158" t="s">
+      <c r="G35" s="180" t="s">
         <v>110</v>
       </c>
-      <c r="H35" s="158"/>
-      <c r="I35" s="158"/>
-      <c r="J35" s="158"/>
-      <c r="K35" s="158"/>
-      <c r="L35" s="158"/>
-      <c r="M35" s="158"/>
+      <c r="H35" s="180"/>
+      <c r="I35" s="180"/>
+      <c r="J35" s="180"/>
+      <c r="K35" s="180"/>
+      <c r="L35" s="180"/>
+      <c r="M35" s="180"/>
       <c r="N35" s="67">
         <v>3</v>
       </c>
       <c r="O35" s="29"/>
       <c r="P35" s="17"/>
     </row>
-    <row r="36" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1">
+    <row r="36" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="17"/>
       <c r="B36" s="29"/>
       <c r="C36" s="68">
         <v>10</v>
       </c>
-      <c r="D36" s="157" t="s">
+      <c r="D36" s="181" t="s">
         <v>108</v>
       </c>
-      <c r="E36" s="206"/>
+      <c r="E36" s="179"/>
       <c r="F36" s="111" t="s">
         <v>111</v>
       </c>
-      <c r="G36" s="158" t="s">
+      <c r="G36" s="180" t="s">
         <v>112</v>
       </c>
-      <c r="H36" s="158"/>
-      <c r="I36" s="158"/>
-      <c r="J36" s="158"/>
-      <c r="K36" s="158"/>
-      <c r="L36" s="158"/>
-      <c r="M36" s="158"/>
+      <c r="H36" s="180"/>
+      <c r="I36" s="180"/>
+      <c r="J36" s="180"/>
+      <c r="K36" s="180"/>
+      <c r="L36" s="180"/>
+      <c r="M36" s="180"/>
       <c r="N36" s="69">
         <v>3</v>
       </c>
       <c r="O36" s="29"/>
       <c r="P36" s="17"/>
     </row>
-    <row r="37" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1">
+    <row r="37" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="17"/>
       <c r="B37" s="29"/>
       <c r="C37" s="66">
         <v>11</v>
       </c>
-      <c r="D37" s="159" t="s">
+      <c r="D37" s="178" t="s">
         <v>108</v>
       </c>
-      <c r="E37" s="206"/>
+      <c r="E37" s="179"/>
       <c r="F37" s="111" t="s">
         <v>113</v>
       </c>
-      <c r="G37" s="158" t="s">
+      <c r="G37" s="180" t="s">
         <v>114</v>
       </c>
-      <c r="H37" s="158"/>
-      <c r="I37" s="158"/>
-      <c r="J37" s="158"/>
-      <c r="K37" s="158"/>
-      <c r="L37" s="158"/>
-      <c r="M37" s="158"/>
+      <c r="H37" s="180"/>
+      <c r="I37" s="180"/>
+      <c r="J37" s="180"/>
+      <c r="K37" s="180"/>
+      <c r="L37" s="180"/>
+      <c r="M37" s="180"/>
       <c r="N37" s="67">
         <v>3</v>
       </c>
       <c r="O37" s="29"/>
       <c r="P37" s="17"/>
     </row>
-    <row r="38" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1">
+    <row r="38" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="17"/>
       <c r="B38" s="29"/>
       <c r="C38" s="70">
         <v>1</v>
       </c>
-      <c r="D38" s="146" t="s">
+      <c r="D38" s="182" t="s">
         <v>115</v>
       </c>
-      <c r="E38" s="146"/>
+      <c r="E38" s="182"/>
       <c r="F38" s="112" t="s">
         <v>116</v>
       </c>
-      <c r="G38" s="147" t="s">
+      <c r="G38" s="183" t="s">
         <v>117</v>
       </c>
-      <c r="H38" s="147"/>
-      <c r="I38" s="147"/>
-      <c r="J38" s="147"/>
-      <c r="K38" s="147"/>
-      <c r="L38" s="147"/>
-      <c r="M38" s="147"/>
+      <c r="H38" s="183"/>
+      <c r="I38" s="183"/>
+      <c r="J38" s="183"/>
+      <c r="K38" s="183"/>
+      <c r="L38" s="183"/>
+      <c r="M38" s="183"/>
       <c r="N38" s="71">
         <v>3</v>
       </c>
       <c r="O38" s="29"/>
       <c r="P38" s="17"/>
     </row>
-    <row r="39" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1">
+    <row r="39" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="17"/>
       <c r="B39" s="29"/>
       <c r="C39" s="72">
         <v>2</v>
       </c>
-      <c r="D39" s="148" t="s">
+      <c r="D39" s="184" t="s">
         <v>115</v>
       </c>
-      <c r="E39" s="207"/>
+      <c r="E39" s="185"/>
       <c r="F39" s="114" t="s">
         <v>118</v>
       </c>
-      <c r="G39" s="149" t="s">
+      <c r="G39" s="186" t="s">
         <v>119</v>
       </c>
-      <c r="H39" s="149"/>
-      <c r="I39" s="149"/>
-      <c r="J39" s="149"/>
-      <c r="K39" s="149"/>
-      <c r="L39" s="149"/>
-      <c r="M39" s="149"/>
+      <c r="H39" s="186"/>
+      <c r="I39" s="186"/>
+      <c r="J39" s="186"/>
+      <c r="K39" s="186"/>
+      <c r="L39" s="186"/>
+      <c r="M39" s="186"/>
       <c r="N39" s="73">
         <v>3</v>
       </c>
       <c r="O39" s="29"/>
       <c r="P39" s="17"/>
     </row>
-    <row r="40" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1">
+    <row r="40" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="17"/>
       <c r="B40" s="29"/>
       <c r="C40" s="74">
         <v>3</v>
       </c>
-      <c r="D40" s="150" t="s">
+      <c r="D40" s="187" t="s">
         <v>120</v>
       </c>
-      <c r="E40" s="208"/>
+      <c r="E40" s="188"/>
       <c r="F40" s="112" t="s">
         <v>121</v>
       </c>
-      <c r="G40" s="147" t="s">
+      <c r="G40" s="183" t="s">
         <v>122</v>
       </c>
-      <c r="H40" s="147"/>
-      <c r="I40" s="147"/>
-      <c r="J40" s="147"/>
-      <c r="K40" s="147"/>
-      <c r="L40" s="147"/>
-      <c r="M40" s="147"/>
+      <c r="H40" s="183"/>
+      <c r="I40" s="183"/>
+      <c r="J40" s="183"/>
+      <c r="K40" s="183"/>
+      <c r="L40" s="183"/>
+      <c r="M40" s="183"/>
       <c r="N40" s="75">
         <v>3</v>
       </c>
       <c r="O40" s="29"/>
       <c r="P40" s="17"/>
     </row>
-    <row r="41" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1">
+    <row r="41" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="17"/>
       <c r="B41" s="29"/>
       <c r="C41" s="76">
         <v>4</v>
       </c>
-      <c r="D41" s="151" t="s">
+      <c r="D41" s="189" t="s">
         <v>123</v>
       </c>
-      <c r="E41" s="207"/>
+      <c r="E41" s="185"/>
       <c r="F41" s="114" t="s">
         <v>124</v>
       </c>
-      <c r="G41" s="149" t="s">
+      <c r="G41" s="186" t="s">
         <v>125</v>
       </c>
-      <c r="H41" s="149"/>
-      <c r="I41" s="149"/>
-      <c r="J41" s="149"/>
-      <c r="K41" s="149"/>
-      <c r="L41" s="149"/>
-      <c r="M41" s="149"/>
+      <c r="H41" s="186"/>
+      <c r="I41" s="186"/>
+      <c r="J41" s="186"/>
+      <c r="K41" s="186"/>
+      <c r="L41" s="186"/>
+      <c r="M41" s="186"/>
       <c r="N41" s="77">
         <v>3</v>
       </c>
       <c r="O41" s="29"/>
       <c r="P41" s="17"/>
     </row>
-    <row r="42" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1">
+    <row r="42" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="17"/>
       <c r="B42" s="29"/>
       <c r="C42" s="70">
         <v>5</v>
       </c>
-      <c r="D42" s="146" t="s">
+      <c r="D42" s="182" t="s">
         <v>126</v>
       </c>
-      <c r="E42" s="209"/>
+      <c r="E42" s="194"/>
       <c r="F42" s="112" t="s">
         <v>126</v>
       </c>
-      <c r="G42" s="147" t="s">
+      <c r="G42" s="183" t="s">
         <v>127</v>
       </c>
-      <c r="H42" s="147"/>
-      <c r="I42" s="147"/>
-      <c r="J42" s="147"/>
-      <c r="K42" s="147"/>
-      <c r="L42" s="147"/>
-      <c r="M42" s="147"/>
+      <c r="H42" s="183"/>
+      <c r="I42" s="183"/>
+      <c r="J42" s="183"/>
+      <c r="K42" s="183"/>
+      <c r="L42" s="183"/>
+      <c r="M42" s="183"/>
       <c r="N42" s="71">
         <v>3</v>
       </c>
       <c r="O42" s="29"/>
       <c r="P42" s="17"/>
     </row>
-    <row r="43" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1">
+    <row r="43" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="17"/>
       <c r="B43" s="29"/>
       <c r="C43" s="72">
         <v>6</v>
       </c>
-      <c r="D43" s="148" t="s">
+      <c r="D43" s="184" t="s">
         <v>126</v>
       </c>
-      <c r="E43" s="207"/>
+      <c r="E43" s="185"/>
       <c r="F43" s="114" t="s">
         <v>128</v>
       </c>
-      <c r="G43" s="149" t="s">
+      <c r="G43" s="186" t="s">
         <v>129</v>
       </c>
-      <c r="H43" s="149"/>
-      <c r="I43" s="149"/>
-      <c r="J43" s="149"/>
-      <c r="K43" s="149"/>
-      <c r="L43" s="149"/>
-      <c r="M43" s="149"/>
+      <c r="H43" s="186"/>
+      <c r="I43" s="186"/>
+      <c r="J43" s="186"/>
+      <c r="K43" s="186"/>
+      <c r="L43" s="186"/>
+      <c r="M43" s="186"/>
       <c r="N43" s="73">
         <v>3</v>
       </c>
       <c r="O43" s="29"/>
       <c r="P43" s="17"/>
     </row>
-    <row r="44" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1">
+    <row r="44" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="17"/>
       <c r="B44" s="29"/>
       <c r="C44" s="74">
         <v>7</v>
       </c>
-      <c r="D44" s="150" t="s">
+      <c r="D44" s="187" t="s">
         <v>130</v>
       </c>
-      <c r="E44" s="208"/>
+      <c r="E44" s="188"/>
       <c r="F44" s="112" t="s">
         <v>131</v>
       </c>
-      <c r="G44" s="147" t="s">
+      <c r="G44" s="183" t="s">
         <v>132</v>
       </c>
-      <c r="H44" s="147"/>
-      <c r="I44" s="147"/>
-      <c r="J44" s="147"/>
-      <c r="K44" s="147"/>
-      <c r="L44" s="147"/>
-      <c r="M44" s="147"/>
+      <c r="H44" s="183"/>
+      <c r="I44" s="183"/>
+      <c r="J44" s="183"/>
+      <c r="K44" s="183"/>
+      <c r="L44" s="183"/>
+      <c r="M44" s="183"/>
       <c r="N44" s="75">
         <v>3</v>
       </c>
       <c r="O44" s="29"/>
       <c r="P44" s="17"/>
     </row>
-    <row r="45" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1">
+    <row r="45" spans="1:16" s="59" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="17"/>
       <c r="B45" s="29"/>
       <c r="C45" s="76">
         <v>8</v>
       </c>
-      <c r="D45" s="151" t="s">
+      <c r="D45" s="189" t="s">
         <v>130</v>
       </c>
-      <c r="E45" s="207"/>
+      <c r="E45" s="185"/>
       <c r="F45" s="114" t="s">
         <v>133</v>
       </c>
-      <c r="G45" s="149" t="s">
+      <c r="G45" s="186" t="s">
         <v>134</v>
       </c>
-      <c r="H45" s="149"/>
-      <c r="I45" s="149"/>
-      <c r="J45" s="149"/>
-      <c r="K45" s="149"/>
-      <c r="L45" s="149"/>
-      <c r="M45" s="149"/>
+      <c r="H45" s="186"/>
+      <c r="I45" s="186"/>
+      <c r="J45" s="186"/>
+      <c r="K45" s="186"/>
+      <c r="L45" s="186"/>
+      <c r="M45" s="186"/>
       <c r="N45" s="77">
         <v>3</v>
       </c>
       <c r="O45" s="29"/>
       <c r="P45" s="17"/>
     </row>
-    <row r="46" spans="1:16" s="59" customFormat="1" ht="13.9">
+    <row r="46" spans="1:16" s="59" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="17"/>
       <c r="B46" s="29"/>
       <c r="C46" s="29"/>
@@ -3955,7 +3955,7 @@
       <c r="O46" s="29"/>
       <c r="P46" s="17"/>
     </row>
-    <row r="47" spans="1:16" s="59" customFormat="1" ht="13.9">
+    <row r="47" spans="1:16" s="59" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="17"/>
       <c r="B47" s="17"/>
       <c r="C47" s="17"/>
@@ -3973,14 +3973,14 @@
       <c r="O47" s="17"/>
       <c r="P47" s="17"/>
     </row>
-    <row r="48" spans="1:16" s="59" customFormat="1" ht="23.45">
+    <row r="48" spans="1:16" s="59" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A48" s="17"/>
       <c r="B48" s="32"/>
-      <c r="C48" s="202" t="s">
+      <c r="C48" s="152" t="s">
         <v>135</v>
       </c>
-      <c r="D48" s="203"/>
-      <c r="E48" s="203"/>
+      <c r="D48" s="153"/>
+      <c r="E48" s="153"/>
       <c r="F48" s="27"/>
       <c r="G48" s="18"/>
       <c r="H48" s="18"/>
@@ -3993,7 +3993,7 @@
       <c r="O48" s="18"/>
       <c r="P48" s="17"/>
     </row>
-    <row r="49" spans="1:16" s="59" customFormat="1" ht="13.9">
+    <row r="49" spans="1:16" s="59" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="17"/>
       <c r="B49" s="32"/>
       <c r="C49" s="33" t="s">
@@ -4003,23 +4003,23 @@
         <v>136</v>
       </c>
       <c r="E49" s="115"/>
-      <c r="F49" s="152" t="s">
+      <c r="F49" s="193" t="s">
         <v>137</v>
       </c>
-      <c r="G49" s="203"/>
-      <c r="H49" s="203"/>
-      <c r="I49" s="203"/>
-      <c r="J49" s="153" t="s">
+      <c r="G49" s="153"/>
+      <c r="H49" s="153"/>
+      <c r="I49" s="153"/>
+      <c r="J49" s="160" t="s">
         <v>138</v>
       </c>
-      <c r="K49" s="203"/>
-      <c r="L49" s="203"/>
-      <c r="M49" s="203"/>
-      <c r="N49" s="203"/>
+      <c r="K49" s="153"/>
+      <c r="L49" s="153"/>
+      <c r="M49" s="153"/>
+      <c r="N49" s="153"/>
       <c r="O49" s="18"/>
       <c r="P49" s="17"/>
     </row>
-    <row r="50" spans="1:16" s="59" customFormat="1" ht="49.35" customHeight="1">
+    <row r="50" spans="1:16" s="59" customFormat="1" ht="49.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="17"/>
       <c r="B50" s="34"/>
       <c r="C50" s="35">
@@ -4029,23 +4029,23 @@
         <v>139</v>
       </c>
       <c r="E50" s="117"/>
-      <c r="F50" s="154" t="s">
+      <c r="F50" s="190" t="s">
         <v>140</v>
       </c>
-      <c r="G50" s="155"/>
-      <c r="H50" s="155"/>
-      <c r="I50" s="155"/>
-      <c r="J50" s="154" t="s">
+      <c r="G50" s="191"/>
+      <c r="H50" s="191"/>
+      <c r="I50" s="191"/>
+      <c r="J50" s="190" t="s">
         <v>141</v>
       </c>
-      <c r="K50" s="155"/>
-      <c r="L50" s="155"/>
-      <c r="M50" s="155"/>
-      <c r="N50" s="155"/>
+      <c r="K50" s="191"/>
+      <c r="L50" s="191"/>
+      <c r="M50" s="191"/>
+      <c r="N50" s="191"/>
       <c r="O50" s="18"/>
       <c r="P50" s="17"/>
     </row>
-    <row r="51" spans="1:16" s="59" customFormat="1" ht="47.45" customHeight="1">
+    <row r="51" spans="1:16" s="59" customFormat="1" ht="47.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="17"/>
       <c r="B51" s="34"/>
       <c r="C51" s="37">
@@ -4055,23 +4055,23 @@
         <v>142</v>
       </c>
       <c r="E51" s="116"/>
-      <c r="F51" s="156" t="s">
+      <c r="F51" s="192" t="s">
         <v>143</v>
       </c>
-      <c r="G51" s="155"/>
-      <c r="H51" s="155"/>
-      <c r="I51" s="155"/>
-      <c r="J51" s="156" t="s">
+      <c r="G51" s="191"/>
+      <c r="H51" s="191"/>
+      <c r="I51" s="191"/>
+      <c r="J51" s="192" t="s">
         <v>144</v>
       </c>
-      <c r="K51" s="155"/>
-      <c r="L51" s="155"/>
-      <c r="M51" s="155"/>
-      <c r="N51" s="155"/>
+      <c r="K51" s="191"/>
+      <c r="L51" s="191"/>
+      <c r="M51" s="191"/>
+      <c r="N51" s="191"/>
       <c r="O51" s="18"/>
       <c r="P51" s="17"/>
     </row>
-    <row r="52" spans="1:16" s="59" customFormat="1" ht="42" customHeight="1">
+    <row r="52" spans="1:16" s="59" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="17"/>
       <c r="B52" s="34"/>
       <c r="C52" s="35">
@@ -4081,23 +4081,23 @@
         <v>145</v>
       </c>
       <c r="E52" s="117"/>
-      <c r="F52" s="154" t="s">
+      <c r="F52" s="190" t="s">
         <v>146</v>
       </c>
-      <c r="G52" s="155"/>
-      <c r="H52" s="155"/>
-      <c r="I52" s="155"/>
-      <c r="J52" s="154" t="s">
+      <c r="G52" s="191"/>
+      <c r="H52" s="191"/>
+      <c r="I52" s="191"/>
+      <c r="J52" s="190" t="s">
         <v>147</v>
       </c>
-      <c r="K52" s="155"/>
-      <c r="L52" s="155"/>
-      <c r="M52" s="155"/>
-      <c r="N52" s="155"/>
+      <c r="K52" s="191"/>
+      <c r="L52" s="191"/>
+      <c r="M52" s="191"/>
+      <c r="N52" s="191"/>
       <c r="O52" s="18"/>
       <c r="P52" s="17"/>
     </row>
-    <row r="53" spans="1:16" s="59" customFormat="1" ht="42.6" customHeight="1">
+    <row r="53" spans="1:16" s="59" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="17"/>
       <c r="B53" s="34"/>
       <c r="C53" s="37">
@@ -4107,23 +4107,23 @@
         <v>148</v>
       </c>
       <c r="E53" s="116"/>
-      <c r="F53" s="156" t="s">
+      <c r="F53" s="192" t="s">
         <v>149</v>
       </c>
-      <c r="G53" s="155"/>
-      <c r="H53" s="155"/>
-      <c r="I53" s="155"/>
-      <c r="J53" s="156" t="s">
+      <c r="G53" s="191"/>
+      <c r="H53" s="191"/>
+      <c r="I53" s="191"/>
+      <c r="J53" s="192" t="s">
         <v>150</v>
       </c>
-      <c r="K53" s="155"/>
-      <c r="L53" s="155"/>
-      <c r="M53" s="155"/>
-      <c r="N53" s="155"/>
+      <c r="K53" s="191"/>
+      <c r="L53" s="191"/>
+      <c r="M53" s="191"/>
+      <c r="N53" s="191"/>
       <c r="O53" s="18"/>
       <c r="P53" s="17"/>
     </row>
-    <row r="54" spans="1:16" s="59" customFormat="1" ht="36" customHeight="1">
+    <row r="54" spans="1:16" s="59" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="17"/>
       <c r="B54" s="34"/>
       <c r="C54" s="35">
@@ -4133,23 +4133,23 @@
         <v>151</v>
       </c>
       <c r="E54" s="117"/>
-      <c r="F54" s="154" t="s">
+      <c r="F54" s="190" t="s">
         <v>152</v>
       </c>
-      <c r="G54" s="155"/>
-      <c r="H54" s="155"/>
-      <c r="I54" s="155"/>
-      <c r="J54" s="154" t="s">
+      <c r="G54" s="191"/>
+      <c r="H54" s="191"/>
+      <c r="I54" s="191"/>
+      <c r="J54" s="190" t="s">
         <v>153</v>
       </c>
-      <c r="K54" s="155"/>
-      <c r="L54" s="155"/>
-      <c r="M54" s="155"/>
-      <c r="N54" s="155"/>
+      <c r="K54" s="191"/>
+      <c r="L54" s="191"/>
+      <c r="M54" s="191"/>
+      <c r="N54" s="191"/>
       <c r="O54" s="18"/>
       <c r="P54" s="17"/>
     </row>
-    <row r="55" spans="1:16" s="59" customFormat="1" ht="13.9">
+    <row r="55" spans="1:16" s="59" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="17"/>
       <c r="B55" s="18"/>
       <c r="C55" s="18"/>
@@ -4167,7 +4167,7 @@
       <c r="O55" s="18"/>
       <c r="P55" s="17"/>
     </row>
-    <row r="56" spans="1:16" s="59" customFormat="1" ht="13.9">
+    <row r="56" spans="1:16" s="59" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="17"/>
       <c r="B56" s="17"/>
       <c r="C56" s="17"/>
@@ -4200,19 +4200,56 @@
     <protectedRange algorithmName="SHA-512" hashValue="NcQe0VjxFnxU9SziGkmWOoYUYoQ0T62vv+WqFE1sowJD2+jDiq1RKEMS6wObDPCk433k/JG1CTU3j62rwNOzdg==" saltValue="OlYFZTFPx5QDCqKlqXj8fw==" spinCount="100000" sqref="F21:K21" name="Range1_2_1_6"/>
   </protectedRanges>
   <mergeCells count="77">
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:K20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="C13:C17"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:K18"/>
-    <mergeCell ref="D13:K13"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="G42:M42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="G43:M43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="G44:M44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="G45:M45"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="J49:N49"/>
+    <mergeCell ref="F54:I54"/>
+    <mergeCell ref="J54:N54"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="J50:N50"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="J51:N51"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="J52:N52"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="J53:N53"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="G39:M39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="G40:M40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="G41:M41"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="G36:M36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="G37:M37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="G38:M38"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="G34:K34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="G35:M35"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D22:K22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:K24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D28:K28"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:I26"/>
+    <mergeCell ref="D27:E27"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="J3:K3"/>
@@ -4227,56 +4264,19 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D22:K22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:K24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D28:K28"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:I26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="G34:K34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="G35:M35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="G36:M36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="G37:M37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="G38:M38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="G39:M39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="G40:M40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="G41:M41"/>
-    <mergeCell ref="F54:I54"/>
-    <mergeCell ref="J54:N54"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="J50:N50"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="J51:N51"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="J52:N52"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="J53:N53"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="G45:M45"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="J49:N49"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="G42:M42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="G43:M43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="G44:M44"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:K20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="C13:C17"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:K18"/>
+    <mergeCell ref="D13:K13"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D15:E15"/>
   </mergeCells>
   <conditionalFormatting sqref="L29:L30">
     <cfRule type="cellIs" dxfId="27" priority="42" operator="equal">
@@ -4393,7 +4393,7 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="13.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="78"/>
     <col min="2" max="2" width="23.85546875" style="78" customWidth="1"/>
@@ -4406,50 +4406,50 @@
     <col min="9" max="16384" width="8.85546875" style="78"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" s="193" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="202" t="s">
         <v>154</v>
       </c>
-      <c r="B1" s="194"/>
-      <c r="C1" s="194"/>
-      <c r="D1" s="194"/>
-      <c r="E1" s="194"/>
-      <c r="F1" s="194"/>
-      <c r="G1" s="194"/>
-      <c r="H1" s="195"/>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="196"/>
-      <c r="B2" s="197"/>
-      <c r="C2" s="197"/>
-      <c r="D2" s="197"/>
-      <c r="E2" s="197"/>
-      <c r="F2" s="197"/>
-      <c r="G2" s="197"/>
-      <c r="H2" s="198"/>
-    </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A3" s="191" t="s">
+      <c r="B1" s="203"/>
+      <c r="C1" s="203"/>
+      <c r="D1" s="203"/>
+      <c r="E1" s="203"/>
+      <c r="F1" s="203"/>
+      <c r="G1" s="203"/>
+      <c r="H1" s="204"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="205"/>
+      <c r="B2" s="206"/>
+      <c r="C2" s="206"/>
+      <c r="D2" s="206"/>
+      <c r="E2" s="206"/>
+      <c r="F2" s="206"/>
+      <c r="G2" s="206"/>
+      <c r="H2" s="207"/>
+    </row>
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="200" t="s">
         <v>103</v>
       </c>
-      <c r="B3" s="192"/>
+      <c r="B3" s="201"/>
       <c r="C3" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="188" t="s">
+      <c r="D3" s="197" t="s">
         <v>135</v>
       </c>
-      <c r="E3" s="189"/>
-      <c r="F3" s="189"/>
-      <c r="G3" s="189"/>
-      <c r="H3" s="190"/>
-      <c r="K3" s="187"/>
-      <c r="L3" s="210"/>
-      <c r="M3" s="210"/>
-      <c r="N3" s="210"/>
+      <c r="E3" s="198"/>
+      <c r="F3" s="198"/>
+      <c r="G3" s="198"/>
+      <c r="H3" s="199"/>
+      <c r="K3" s="195"/>
+      <c r="L3" s="196"/>
+      <c r="M3" s="196"/>
+      <c r="N3" s="196"/>
       <c r="O3" s="100"/>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="99"/>
       <c r="B4" s="98"/>
       <c r="C4" s="98"/>
@@ -4469,7 +4469,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="26.45">
+    <row r="5" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="91"/>
       <c r="D5" s="94" t="s">
         <v>155</v>
@@ -4487,7 +4487,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="91"/>
       <c r="D6" s="90"/>
       <c r="E6" s="89"/>
@@ -4495,7 +4495,7 @@
       <c r="G6" s="89"/>
       <c r="H6" s="88"/>
     </row>
-    <row r="7" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1">
+    <row r="7" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="105">
         <v>1</v>
       </c>
@@ -4521,7 +4521,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1">
+    <row r="8" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="105">
         <v>2</v>
       </c>
@@ -4545,7 +4545,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1">
+    <row r="9" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="133">
         <v>3</v>
       </c>
@@ -4571,7 +4571,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1">
+    <row r="10" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="142">
         <v>4</v>
       </c>
@@ -4595,7 +4595,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1">
+    <row r="11" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="102">
         <v>5</v>
       </c>
@@ -4619,7 +4619,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1">
+    <row r="12" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="102">
         <v>6</v>
       </c>
@@ -4645,7 +4645,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1">
+    <row r="13" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="102">
         <v>7</v>
       </c>
@@ -4669,7 +4669,7 @@
       </c>
       <c r="H13" s="101"/>
     </row>
-    <row r="14" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1">
+    <row r="14" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="102">
         <v>8</v>
       </c>
@@ -4693,7 +4693,7 @@
       </c>
       <c r="H14" s="101"/>
     </row>
-    <row r="15" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1">
+    <row r="15" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="87">
         <v>9</v>
       </c>
@@ -4717,7 +4717,7 @@
       </c>
       <c r="H15" s="85"/>
     </row>
-    <row r="16" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1">
+    <row r="16" spans="1:15" s="84" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="87">
         <v>10</v>
       </c>
@@ -4743,7 +4743,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="80.099999999999994" customHeight="1">
+    <row r="17" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="83">
         <v>11</v>
       </c>
@@ -4789,21 +4789,21 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="7" max="7" width="18.140625" customWidth="1"/>
     <col min="9" max="9" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:20" ht="26.45">
+    <row r="2" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="B2" s="201" t="s">
+      <c r="B2" s="210" t="s">
         <v>170</v>
       </c>
-      <c r="C2" s="205"/>
-      <c r="D2" s="205"/>
+      <c r="C2" s="161"/>
+      <c r="D2" s="161"/>
       <c r="G2" s="4"/>
       <c r="H2" s="1" t="s">
         <v>171</v>
@@ -4824,7 +4824,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="13.9">
+    <row r="3" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B3" s="119"/>
       <c r="C3" s="119"/>
       <c r="D3" s="119"/>
@@ -4844,7 +4844,7 @@
       <c r="S3" s="2"/>
       <c r="T3" s="4"/>
     </row>
-    <row r="4" spans="1:20" ht="13.9">
+    <row r="4" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B4" s="119"/>
       <c r="C4" s="119"/>
       <c r="D4" s="119"/>
@@ -4864,12 +4864,12 @@
       <c r="S4" s="2"/>
       <c r="T4" s="4"/>
     </row>
-    <row r="5" spans="1:20" ht="184.9">
-      <c r="B5" s="199" t="s">
+    <row r="5" spans="1:20" ht="191.25" x14ac:dyDescent="0.2">
+      <c r="B5" s="208" t="s">
         <v>177</v>
       </c>
-      <c r="C5" s="205"/>
-      <c r="D5" s="205"/>
+      <c r="C5" s="161"/>
+      <c r="D5" s="161"/>
       <c r="F5" s="10">
         <v>6.1</v>
       </c>
@@ -4920,7 +4920,7 @@
       </c>
       <c r="T5" s="4"/>
     </row>
-    <row r="6" spans="1:20" ht="105.6">
+    <row r="6" spans="1:20" ht="127.5" x14ac:dyDescent="0.2">
       <c r="B6" s="119"/>
       <c r="C6" s="119"/>
       <c r="D6" s="119"/>
@@ -4951,12 +4951,12 @@
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
     </row>
-    <row r="7" spans="1:20" ht="79.900000000000006">
-      <c r="B7" s="199" t="s">
+    <row r="7" spans="1:20" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="B7" s="208" t="s">
         <v>191</v>
       </c>
-      <c r="C7" s="205"/>
-      <c r="D7" s="205"/>
+      <c r="C7" s="161"/>
+      <c r="D7" s="161"/>
       <c r="F7" s="10">
         <v>6.2</v>
       </c>
@@ -5007,12 +5007,12 @@
       </c>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20" ht="66.599999999999994">
-      <c r="B8" s="199" t="s">
+    <row r="8" spans="1:20" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="B8" s="208" t="s">
         <v>199</v>
       </c>
-      <c r="C8" s="205"/>
-      <c r="D8" s="205"/>
+      <c r="C8" s="161"/>
+      <c r="D8" s="161"/>
       <c r="G8" s="4"/>
       <c r="H8" s="9" t="s">
         <v>185</v>
@@ -5040,7 +5040,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:20" ht="13.15">
+    <row r="9" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G9" s="10"/>
       <c r="H9" s="4"/>
       <c r="I9" s="10"/>
@@ -5048,7 +5048,7 @@
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
     </row>
-    <row r="10" spans="1:20" ht="13.15">
+    <row r="10" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G10" s="10"/>
       <c r="H10" s="4"/>
       <c r="I10" s="10"/>
@@ -5057,7 +5057,7 @@
       <c r="L10" s="10"/>
       <c r="M10" s="11"/>
     </row>
-    <row r="11" spans="1:20" ht="13.15">
+    <row r="11" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G11" s="10"/>
       <c r="H11" s="4"/>
       <c r="I11" s="10"/>
@@ -5066,7 +5066,7 @@
       <c r="L11" s="10"/>
       <c r="M11" s="11"/>
     </row>
-    <row r="12" spans="1:20" ht="13.15">
+    <row r="12" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G12" s="10"/>
       <c r="H12" s="4"/>
       <c r="I12" s="10"/>
@@ -5075,10 +5075,10 @@
       <c r="L12" s="10"/>
       <c r="M12" s="11"/>
     </row>
-    <row r="13" spans="1:20" ht="13.9">
-      <c r="B13" s="200"/>
-      <c r="C13" s="205"/>
-      <c r="D13" s="205"/>
+    <row r="13" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B13" s="209"/>
+      <c r="C13" s="161"/>
+      <c r="D13" s="161"/>
       <c r="G13" s="10"/>
       <c r="H13" s="4" t="s">
         <v>205</v>
@@ -5099,12 +5099,12 @@
         <v>210</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="70.5" customHeight="1">
-      <c r="B14" s="199" t="s">
+    <row r="14" spans="1:20" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="208" t="s">
         <v>211</v>
       </c>
-      <c r="C14" s="205"/>
-      <c r="D14" s="205"/>
+      <c r="C14" s="161"/>
+      <c r="D14" s="161"/>
       <c r="F14" s="10">
         <v>3.1</v>
       </c>
@@ -5152,7 +5152,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="66.75" customHeight="1">
+    <row r="15" spans="1:20" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="13"/>
       <c r="G15" s="12" t="s">
         <v>217</v>
@@ -5176,7 +5176,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="13.15">
+    <row r="16" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G16" s="10"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
@@ -5185,7 +5185,7 @@
       <c r="L16" s="4"/>
       <c r="M16" s="14"/>
     </row>
-    <row r="17" spans="2:19" ht="13.15">
+    <row r="17" spans="2:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G17" s="10"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
@@ -5194,12 +5194,12 @@
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
     </row>
-    <row r="18" spans="2:19" ht="251.45">
-      <c r="B18" s="199" t="s">
+    <row r="18" spans="2:19" ht="255" x14ac:dyDescent="0.2">
+      <c r="B18" s="208" t="s">
         <v>223</v>
       </c>
-      <c r="C18" s="205"/>
-      <c r="D18" s="205"/>
+      <c r="C18" s="161"/>
+      <c r="D18" s="161"/>
       <c r="F18" s="10">
         <v>3.2</v>
       </c>
@@ -5247,7 +5247,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="19" spans="2:19" ht="132">
+    <row r="19" spans="2:19" ht="127.5" x14ac:dyDescent="0.2">
       <c r="G19" s="10"/>
       <c r="H19" s="9" t="s">
         <v>185</v>
@@ -5262,7 +5262,7 @@
       </c>
       <c r="M19" s="4"/>
     </row>
-    <row r="20" spans="2:19" ht="13.15">
+    <row r="20" spans="2:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G20" s="10"/>
       <c r="H20" s="4"/>
       <c r="I20" s="10"/>
@@ -5271,7 +5271,7 @@
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
     </row>
-    <row r="21" spans="2:19" ht="13.15">
+    <row r="21" spans="2:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
@@ -5280,7 +5280,7 @@
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
     </row>
-    <row r="22" spans="2:19" ht="13.15">
+    <row r="22" spans="2:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
@@ -5289,7 +5289,7 @@
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
     </row>
-    <row r="24" spans="2:19" ht="13.15">
+    <row r="24" spans="2:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="H24" s="10" t="s">
         <v>231</v>
       </c>
@@ -5309,12 +5309,12 @@
         <v>234</v>
       </c>
     </row>
-    <row r="25" spans="2:19" ht="290.45">
-      <c r="B25" s="200" t="s">
+    <row r="25" spans="2:19" ht="280.5" x14ac:dyDescent="0.2">
+      <c r="B25" s="209" t="s">
         <v>235</v>
       </c>
-      <c r="C25" s="205"/>
-      <c r="D25" s="205"/>
+      <c r="C25" s="161"/>
+      <c r="D25" s="161"/>
       <c r="G25" s="10" t="s">
         <v>236</v>
       </c>
@@ -5337,7 +5337,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="26" spans="2:19" ht="13.15">
+    <row r="26" spans="2:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G26" s="10" t="s">
         <v>243</v>
       </c>
@@ -5359,14 +5359,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bd38d267-56bb-4e22-b975-199a06fd69fa">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d8c712e5-67fc-4595-93cb-a4164dd8eff3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5625,22 +5623,50 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bd38d267-56bb-4e22-b975-199a06fd69fa">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d8c712e5-67fc-4595-93cb-a4164dd8eff3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D98D897-3D5D-4CF5-A274-8B2E15AE73B2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BB72468-B9EB-412A-8D55-6151E9A308C0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{873E3095-4F4D-4DD9-BAD5-E276899012AF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{873E3095-4F4D-4DD9-BAD5-E276899012AF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bd38d267-56bb-4e22-b975-199a06fd69fa"/>
+    <ds:schemaRef ds:uri="d8c712e5-67fc-4595-93cb-a4164dd8eff3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BB72468-B9EB-412A-8D55-6151E9A308C0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D98D897-3D5D-4CF5-A274-8B2E15AE73B2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bd38d267-56bb-4e22-b975-199a06fd69fa"/>
+    <ds:schemaRef ds:uri="d8c712e5-67fc-4595-93cb-a4164dd8eff3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>